<commit_message>
Updated achievement. Added video example for solution creating.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE07212-4AE6-4AE9-9B6D-2D68874884AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A2B4BE-2F45-4AB2-BECB-AF7B8CD406C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:AQ237"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -877,7 +877,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AG3" s="4" t="e">
-        <f t="shared" ref="AG2:AG42" si="8">MAX(IF(AF3*100&gt;=20,2,0),IF(AF3*100&gt;=40,3,0),IF(AF3*100&gt;=60,4,0),IF(AF3*100&gt;=80,5,0))</f>
+        <f t="shared" ref="AG3:AG42" si="8">MAX(IF(AF3*100&gt;=20,2,0),IF(AF3*100&gt;=40,3,0),IF(AF3*100&gt;=60,4,0),IF(AF3*100&gt;=80,5,0))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AH3" s="1"/>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="AP3" s="4" t="e">
-        <f t="shared" ref="AP2:AP42" si="9">(AG3+AN3+AO3)/3</f>
+        <f t="shared" ref="AP3:AP42" si="9">(AG3+AN3+AO3)/3</f>
         <v>#DIV/0!</v>
       </c>
       <c r="AQ3" s="5"/>
@@ -1810,7 +1810,9 @@
         <v>54</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1828,7 +1830,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
@@ -1844,7 +1846,7 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15" s="1">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update achievement. Change .bat files.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D87D7FB-7639-46E3-9B1D-7E9E546A3A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1956841C-C2D8-42B0-BA1D-8C0220E72127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -766,7 +766,9 @@
       <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -782,7 +784,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f t="shared" ref="T2:T34" si="0">SUM(C2:S2)</f>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="U2" s="9">
         <v>0.1</v>
@@ -800,15 +802,15 @@
       </c>
       <c r="AD2" s="1">
         <f t="shared" ref="AD2:AD34" si="2">T2+AC2</f>
-        <v>2.1</v>
+        <v>3.6</v>
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.95454545454545447</v>
+        <v>1.125</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
@@ -853,7 +855,9 @@
       <c r="E3" s="1">
         <v>1.5</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -869,7 +873,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U3" s="1">
         <v>0</v>
@@ -887,15 +891,15 @@
       </c>
       <c r="AD3" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
@@ -940,7 +944,9 @@
       <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -956,7 +962,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U4" s="9">
         <v>0</v>
@@ -974,15 +980,15 @@
       </c>
       <c r="AD4" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.90909090909090906</v>
+        <v>0.9375</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
@@ -1027,7 +1033,9 @@
       <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1043,7 +1051,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="U5" s="9">
         <v>0.1</v>
@@ -1061,15 +1069,15 @@
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="2"/>
-        <v>2.1</v>
+        <v>3.6</v>
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="4"/>
-        <v>0.95454545454545447</v>
+        <v>1.125</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="5"/>
@@ -1114,7 +1122,9 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1130,7 +1140,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U6" s="9">
         <v>0</v>
@@ -1148,15 +1158,15 @@
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" si="4"/>
-        <v>0.90909090909090906</v>
+        <v>0.9375</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="5"/>
@@ -1201,7 +1211,9 @@
       <c r="E7" s="1">
         <v>1.5</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1217,7 +1229,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U7" s="9">
         <v>0</v>
@@ -1235,15 +1247,15 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
@@ -1288,7 +1300,9 @@
       <c r="E8" s="9">
         <v>1.5</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1304,7 +1318,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U8" s="9">
         <v>0</v>
@@ -1322,15 +1336,15 @@
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE8" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF8" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="5"/>
@@ -1375,7 +1389,9 @@
       <c r="E9" s="9">
         <v>1.5</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1391,7 +1407,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U9" s="1">
         <v>0.2</v>
@@ -1409,15 +1425,15 @@
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="2"/>
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>1.2272727272727273</v>
+        <v>1.3125</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
@@ -1502,11 +1518,11 @@
       </c>
       <c r="AE10" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF10" s="7">
         <f t="shared" si="4"/>
-        <v>1.8636363636363633</v>
+        <v>1.2812499999999998</v>
       </c>
       <c r="AG10" s="4">
         <f t="shared" si="5"/>
@@ -1551,7 +1567,9 @@
       <c r="E11" s="9">
         <v>1.5</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1567,7 +1585,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U11" s="9">
         <v>0</v>
@@ -1585,15 +1603,15 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE11" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF11" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG11" s="4">
         <f t="shared" si="5"/>
@@ -1638,7 +1656,9 @@
       <c r="E12" s="9">
         <v>1.5</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1654,7 +1674,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U12" s="9">
         <v>0</v>
@@ -1672,15 +1692,15 @@
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
@@ -1725,7 +1745,9 @@
       <c r="E13" s="9">
         <v>1.5</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>0.6</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1741,7 +1763,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="U13" s="9">
         <v>0</v>
@@ -1759,15 +1781,15 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="AE13" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF13" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>0.96875</v>
       </c>
       <c r="AG13" s="4">
         <f t="shared" si="5"/>
@@ -1812,7 +1834,9 @@
       <c r="E14" s="1">
         <v>1.5</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1828,7 +1852,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U14" s="9">
         <v>0.2</v>
@@ -1846,15 +1870,15 @@
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="2"/>
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="AE14" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF14" s="7">
         <f t="shared" si="4"/>
-        <v>1.2272727272727273</v>
+        <v>1.3125</v>
       </c>
       <c r="AG14" s="4">
         <f t="shared" si="5"/>
@@ -1899,7 +1923,9 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1915,7 +1941,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="U15" s="9">
         <v>0</v>
@@ -1933,15 +1959,15 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="AE15" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF15" s="7">
         <f t="shared" si="4"/>
-        <v>0.90909090909090906</v>
+        <v>1.09375</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="5"/>
@@ -1986,7 +2012,9 @@
       <c r="E16" s="9">
         <v>1.5</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -2002,7 +2030,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U16" s="9">
         <v>0</v>
@@ -2020,15 +2048,15 @@
       </c>
       <c r="AD16" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE16" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF16" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG16" s="4">
         <f t="shared" si="5"/>
@@ -2073,7 +2101,9 @@
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2089,7 +2119,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="U17" s="9">
         <v>0.1</v>
@@ -2107,15 +2137,15 @@
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="2"/>
-        <v>2.1</v>
+        <v>3.6</v>
       </c>
       <c r="AE17" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF17" s="7">
         <f t="shared" si="4"/>
-        <v>0.95454545454545447</v>
+        <v>1.125</v>
       </c>
       <c r="AG17" s="4">
         <f t="shared" si="5"/>
@@ -2160,7 +2190,9 @@
       <c r="E18" s="1">
         <v>1.5</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2176,7 +2208,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U18" s="9">
         <v>0</v>
@@ -2194,15 +2226,15 @@
       </c>
       <c r="AD18" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE18" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF18" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" si="5"/>
@@ -2247,7 +2279,9 @@
       <c r="E19" s="1">
         <v>1.5</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2263,7 +2297,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U19" s="9">
         <v>0.1</v>
@@ -2281,15 +2315,15 @@
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="2"/>
-        <v>2.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>1.1818181818181817</v>
+        <v>1.2812499999999998</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
@@ -2337,7 +2371,9 @@
       <c r="F20" s="9">
         <v>1.5</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2352,7 +2388,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U20" s="9">
         <v>0.1</v>
@@ -2370,15 +2406,15 @@
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="2"/>
-        <v>4.0999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>1.8636363636363633</v>
+        <v>1.5937499999999998</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
@@ -2423,7 +2459,9 @@
       <c r="E21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1">
+        <v>0.6</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2439,7 +2477,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="U21" s="9">
         <v>0</v>
@@ -2457,15 +2495,15 @@
       </c>
       <c r="AD21" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="AE21" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF21" s="7">
         <f t="shared" si="4"/>
-        <v>0.90909090909090906</v>
+        <v>0.8125</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="5"/>
@@ -2510,7 +2548,9 @@
       <c r="E22" s="1">
         <v>1.5</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2526,7 +2566,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U22" s="1">
         <v>0.1</v>
@@ -2544,15 +2584,15 @@
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="2"/>
-        <v>2.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>1.1818181818181817</v>
+        <v>1.2812499999999998</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
@@ -2597,7 +2637,9 @@
       <c r="E23" s="9">
         <v>1.5</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="9">
+        <v>0.6</v>
+      </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -2613,7 +2655,7 @@
       <c r="S23" s="9"/>
       <c r="T23" s="9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="U23" s="9">
         <v>0</v>
@@ -2631,15 +2673,15 @@
       </c>
       <c r="AD23" s="9">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="AE23" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF23" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>0.96875</v>
       </c>
       <c r="AG23" s="8">
         <f t="shared" si="5"/>
@@ -2720,15 +2762,15 @@
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>0.45454545454545453</v>
+        <v>0.3125</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
@@ -2753,7 +2795,7 @@
       </c>
       <c r="AP24" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AQ24" s="5"/>
     </row>
@@ -2769,7 +2811,9 @@
       <c r="E25" s="1">
         <v>1.5</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2785,7 +2829,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="U25" s="9">
         <v>0.1</v>
@@ -2803,15 +2847,15 @@
       </c>
       <c r="AD25" s="1">
         <f t="shared" si="2"/>
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="AE25" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF25" s="7">
         <f t="shared" si="4"/>
-        <v>1.1818181818181817</v>
+        <v>1.125</v>
       </c>
       <c r="AG25" s="4">
         <f t="shared" si="5"/>
@@ -2856,7 +2900,9 @@
       <c r="E26" s="1">
         <v>1.5</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -2872,7 +2918,7 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U26" s="9">
         <v>0</v>
@@ -2890,15 +2936,15 @@
       </c>
       <c r="AD26" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE26" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF26" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG26" s="4">
         <f t="shared" si="5"/>
@@ -2946,7 +2992,9 @@
       <c r="F27" s="9">
         <v>1.5</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2961,7 +3009,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U27" s="9">
         <v>0.2</v>
@@ -2979,15 +3027,15 @@
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="2"/>
-        <v>4.2</v>
+        <v>5.2</v>
       </c>
       <c r="AE27" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF27" s="7">
         <f t="shared" si="4"/>
-        <v>1.9090909090909089</v>
+        <v>1.625</v>
       </c>
       <c r="AG27" s="4">
         <f t="shared" si="5"/>
@@ -3072,11 +3120,11 @@
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>1.9090909090909089</v>
+        <v>1.3125</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
@@ -3121,7 +3169,9 @@
       <c r="E29" s="1">
         <v>1.5</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -3137,7 +3187,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U29" s="9">
         <v>0</v>
@@ -3155,15 +3205,15 @@
       </c>
       <c r="AD29" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE29" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF29" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG29" s="4">
         <f t="shared" si="5"/>
@@ -3208,7 +3258,9 @@
       <c r="E30" s="1">
         <v>1</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1">
+        <v>0.6</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -3224,7 +3276,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="U30" s="9">
         <v>0</v>
@@ -3242,15 +3294,15 @@
       </c>
       <c r="AD30" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="AE30" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF30" s="7">
         <f t="shared" si="4"/>
-        <v>0.90909090909090906</v>
+        <v>0.8125</v>
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="5"/>
@@ -3335,11 +3387,11 @@
       </c>
       <c r="AE31" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF31" s="7">
         <f t="shared" si="4"/>
-        <v>1.9090909090909089</v>
+        <v>1.3125</v>
       </c>
       <c r="AG31" s="4">
         <f t="shared" si="5"/>
@@ -3384,7 +3436,9 @@
       <c r="E32" s="9">
         <v>1.5</v>
       </c>
-      <c r="F32" s="9"/>
+      <c r="F32" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -3400,7 +3454,7 @@
       <c r="S32" s="9"/>
       <c r="T32" s="9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U32" s="9">
         <v>0.1</v>
@@ -3418,15 +3472,15 @@
       </c>
       <c r="AD32" s="9">
         <f t="shared" si="2"/>
-        <v>2.6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AE32" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF32" s="7">
         <f t="shared" si="4"/>
-        <v>1.1818181818181817</v>
+        <v>1.2812499999999998</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="5"/>
@@ -3471,7 +3525,9 @@
       <c r="E33" s="9">
         <v>1.5</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="F33" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
@@ -3487,7 +3543,7 @@
       <c r="S33" s="9"/>
       <c r="T33" s="9">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U33" s="9">
         <v>0</v>
@@ -3505,15 +3561,15 @@
       </c>
       <c r="AD33" s="9">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
@@ -3558,7 +3614,9 @@
       <c r="E34" s="1">
         <v>1.5</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="9">
+        <v>1.5</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -3574,7 +3632,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="U34" s="9">
         <v>0</v>
@@ -3592,15 +3650,15 @@
       </c>
       <c r="AD34" s="1">
         <f t="shared" si="2"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>1.1363636363636362</v>
+        <v>1.25</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>
@@ -3645,7 +3703,9 @@
       <c r="E35" s="1">
         <v>1</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -3661,7 +3721,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1">
         <f t="shared" ref="T35" si="10">SUM(C35:S35)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U35" s="1">
         <v>0.2</v>
@@ -3679,11 +3739,11 @@
       </c>
       <c r="AD35" s="1">
         <f t="shared" ref="AD35" si="12">T35+AC35</f>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AE35" s="4">
         <f>AD35</f>
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AF35" s="7">
         <f t="shared" ref="AF35" si="13">(AD35/AE35)</f>

</xml_diff>

<commit_message>
Update achievement. Add solution-5.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2518FF57-808D-4A73-823D-CB3275C77800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D36F41-0018-4A40-84FD-A960F68F543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="МК-101" sheetId="1" r:id="rId1"/>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -773,7 +773,9 @@
       <c r="H2" s="1">
         <v>0.6</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1">
+        <v>0.1</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -786,7 +788,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f t="shared" ref="T2:T34" si="0">SUM(C2:S2)</f>
-        <v>4.75</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="U2" s="9">
         <v>0.1</v>
@@ -804,19 +806,19 @@
       </c>
       <c r="AD2" s="1">
         <f t="shared" ref="AD2:AD34" si="2">T2+AC2</f>
-        <v>4.8499999999999996</v>
+        <v>4.9499999999999993</v>
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.9326923076923076</v>
+        <v>0.79838709677419339</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
@@ -841,7 +843,7 @@
       </c>
       <c r="AP2" s="4">
         <f t="shared" ref="AP2:AP34" si="9">(AG2+AN2+AO2)/3</f>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ2" s="5"/>
     </row>
@@ -899,15 +901,15 @@
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>0.89423076923076927</v>
+        <v>0.75</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -932,7 +934,7 @@
       </c>
       <c r="AP3" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ3" s="5"/>
     </row>
@@ -992,15 +994,15 @@
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.81730769230769229</v>
+        <v>0.68548387096774188</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1025,7 +1027,7 @@
       </c>
       <c r="AP4" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ4" s="5"/>
     </row>
@@ -1083,15 +1085,15 @@
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="4"/>
-        <v>0.80769230769230749</v>
+        <v>0.67741935483870952</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -1116,7 +1118,7 @@
       </c>
       <c r="AP5" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ5" s="5"/>
     </row>
@@ -1174,15 +1176,15 @@
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" si="4"/>
-        <v>0.70192307692307687</v>
+        <v>0.58870967741935476</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
@@ -1207,7 +1209,7 @@
       </c>
       <c r="AP6" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="5"/>
     </row>
@@ -1232,7 +1234,9 @@
       <c r="H7" s="1">
         <v>1.5</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1245,7 +1249,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="U7" s="9">
         <v>0</v>
@@ -1263,15 +1267,15 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.1451612903225805</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
@@ -1325,7 +1329,9 @@
       <c r="H8" s="1">
         <v>0.6</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1338,7 +1344,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1">
         <f t="shared" si="0"/>
-        <v>5.25</v>
+        <v>5.85</v>
       </c>
       <c r="U8" s="9">
         <v>0</v>
@@ -1356,15 +1362,15 @@
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="2"/>
-        <v>5.25</v>
+        <v>5.85</v>
       </c>
       <c r="AE8" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF8" s="7">
         <f t="shared" si="4"/>
-        <v>1.0096153846153846</v>
+        <v>0.94354838709677413</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="5"/>
@@ -1451,15 +1457,15 @@
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>0.93269230769230771</v>
+        <v>0.78225806451612911</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
@@ -1484,7 +1490,7 @@
       </c>
       <c r="AP9" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ9" s="5"/>
     </row>
@@ -1544,11 +1550,11 @@
       </c>
       <c r="AE10" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF10" s="7">
         <f t="shared" si="4"/>
-        <v>1.2692307692307692</v>
+        <v>1.064516129032258</v>
       </c>
       <c r="AG10" s="4">
         <f t="shared" si="5"/>
@@ -1637,11 +1643,11 @@
       </c>
       <c r="AE11" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF11" s="7">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.0483870967741935</v>
       </c>
       <c r="AG11" s="4">
         <f t="shared" si="5"/>
@@ -1693,7 +1699,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1708,12 +1714,14 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="U12" s="9">
         <v>0</v>
       </c>
-      <c r="V12" s="1"/>
+      <c r="V12" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
@@ -1722,19 +1730,19 @@
       <c r="AB12" s="1"/>
       <c r="AC12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="2"/>
-        <v>5.6</v>
+        <v>5.8999999999999995</v>
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>1.0769230769230769</v>
+        <v>0.95161290322580638</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
@@ -1788,7 +1796,9 @@
       <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>0.1</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1801,7 +1811,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="U13" s="9">
         <v>0</v>
@@ -1819,19 +1829,19 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="2"/>
-        <v>4.75</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="AE13" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF13" s="7">
         <f t="shared" si="4"/>
-        <v>0.91346153846153844</v>
+        <v>0.782258064516129</v>
       </c>
       <c r="AG13" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
@@ -1856,7 +1866,7 @@
       </c>
       <c r="AP13" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ13" s="5"/>
     </row>
@@ -1879,7 +1889,9 @@
         <v>1</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -1892,12 +1904,14 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U14" s="9">
         <v>0.2</v>
       </c>
-      <c r="V14" s="1"/>
+      <c r="V14" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
@@ -1906,19 +1920,19 @@
       <c r="AB14" s="1"/>
       <c r="AC14" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="2"/>
-        <v>5.2</v>
+        <v>6.3</v>
       </c>
       <c r="AE14" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF14" s="7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>1.0161290322580645</v>
       </c>
       <c r="AG14" s="4">
         <f t="shared" si="5"/>
@@ -2005,11 +2019,11 @@
       </c>
       <c r="AE15" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF15" s="7">
         <f t="shared" si="4"/>
-        <v>0.79807692307692313</v>
+        <v>0.66935483870967749</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="5"/>
@@ -2063,7 +2077,9 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2076,7 +2092,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1">
         <f t="shared" si="0"/>
-        <v>5.65</v>
+        <v>6.25</v>
       </c>
       <c r="U16" s="9">
         <v>0</v>
@@ -2094,15 +2110,15 @@
       </c>
       <c r="AD16" s="1">
         <f t="shared" si="2"/>
-        <v>5.65</v>
+        <v>6.25</v>
       </c>
       <c r="AE16" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF16" s="7">
         <f t="shared" si="4"/>
-        <v>1.0865384615384617</v>
+        <v>1.0080645161290323</v>
       </c>
       <c r="AG16" s="4">
         <f t="shared" si="5"/>
@@ -2189,15 +2205,15 @@
       </c>
       <c r="AE17" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF17" s="7">
         <f t="shared" si="4"/>
-        <v>0.81730769230769229</v>
+        <v>0.68548387096774188</v>
       </c>
       <c r="AG17" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
@@ -2222,7 +2238,7 @@
       </c>
       <c r="AP17" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ17" s="5"/>
     </row>
@@ -2280,15 +2296,15 @@
       </c>
       <c r="AE18" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF18" s="7">
         <f t="shared" si="4"/>
-        <v>0.89423076923076927</v>
+        <v>0.75</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2313,7 +2329,7 @@
       </c>
       <c r="AP18" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ18" s="5"/>
     </row>
@@ -2338,7 +2354,9 @@
       <c r="H19" s="1">
         <v>0.6</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2351,12 +2369,14 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1">
         <f t="shared" si="0"/>
-        <v>5.6</v>
+        <v>6.1999999999999993</v>
       </c>
       <c r="U19" s="9">
         <v>0.1</v>
       </c>
-      <c r="V19" s="1"/>
+      <c r="V19" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -2365,19 +2385,19 @@
       <c r="AB19" s="1"/>
       <c r="AC19" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="2"/>
-        <v>5.6999999999999993</v>
+        <v>6.3999999999999995</v>
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>1.096153846153846</v>
+        <v>1.032258064516129</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
@@ -2451,7 +2471,9 @@
       <c r="U20" s="9">
         <v>0.1</v>
       </c>
-      <c r="V20" s="1"/>
+      <c r="V20" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
@@ -2460,19 +2482,19 @@
       <c r="AB20" s="1"/>
       <c r="AC20" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="2"/>
-        <v>8.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>1.5576923076923075</v>
+        <v>1.3225806451612903</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
@@ -2559,15 +2581,15 @@
       </c>
       <c r="AE21" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF21" s="7">
         <f t="shared" si="4"/>
-        <v>0.70192307692307687</v>
+        <v>0.58870967741935476</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
@@ -2592,7 +2614,7 @@
       </c>
       <c r="AP21" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ21" s="5"/>
     </row>
@@ -2617,7 +2639,9 @@
       <c r="H22" s="1">
         <v>1.5</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2630,12 +2654,14 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="U22" s="1">
         <v>0.1</v>
       </c>
-      <c r="V22" s="1"/>
+      <c r="V22" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
@@ -2644,19 +2670,19 @@
       <c r="AB22" s="1"/>
       <c r="AC22" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="2"/>
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>1.2692307692307692</v>
+        <v>1.1774193548387095</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
@@ -2741,15 +2767,15 @@
       </c>
       <c r="AE23" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF23" s="7">
         <f t="shared" si="4"/>
-        <v>0.67307692307692302</v>
+        <v>0.56451612903225801</v>
       </c>
       <c r="AG23" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH23" s="9"/>
       <c r="AI23" s="9"/>
@@ -2774,7 +2800,7 @@
       </c>
       <c r="AP23" s="8">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ23" s="5"/>
     </row>
@@ -2799,7 +2825,9 @@
       <c r="H24" s="1">
         <v>1.5</v>
       </c>
-      <c r="I24" s="1"/>
+      <c r="I24" s="1">
+        <v>1.5</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -2812,7 +2840,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="U24" s="9">
         <v>0</v>
@@ -2830,15 +2858,15 @@
       </c>
       <c r="AD24" s="1">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>1.1538461538461537</v>
+        <v>1.2096774193548387</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
@@ -2927,11 +2955,11 @@
       </c>
       <c r="AE25" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF25" s="7">
         <f t="shared" si="4"/>
-        <v>1.0096153846153846</v>
+        <v>0.84677419354838712</v>
       </c>
       <c r="AG25" s="4">
         <f t="shared" si="5"/>
@@ -2985,7 +3013,9 @@
       <c r="H26" s="1">
         <v>1.5</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2998,12 +3028,14 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="U26" s="9">
         <v>0</v>
       </c>
-      <c r="V26" s="1"/>
+      <c r="V26" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
@@ -3012,19 +3044,19 @@
       <c r="AB26" s="1"/>
       <c r="AC26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD26" s="1">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>7.6</v>
       </c>
       <c r="AE26" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF26" s="7">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.225806451612903</v>
       </c>
       <c r="AG26" s="4">
         <f t="shared" si="5"/>
@@ -3078,7 +3110,9 @@
       <c r="H27" s="1">
         <v>1.5</v>
       </c>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1">
+        <v>1.5</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -3091,12 +3125,14 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="U27" s="9">
         <v>0.2</v>
       </c>
-      <c r="V27" s="1"/>
+      <c r="V27" s="1">
+        <v>0.2</v>
+      </c>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
@@ -3105,48 +3141,50 @@
       <c r="AB27" s="1"/>
       <c r="AC27" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="2"/>
-        <v>6.7</v>
+        <v>8.4</v>
       </c>
       <c r="AE27" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF27" s="7">
         <f t="shared" si="4"/>
-        <v>1.2884615384615385</v>
+        <v>1.3548387096774195</v>
       </c>
       <c r="AG27" s="4">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="AH27" s="1"/>
+      <c r="AH27" s="1">
+        <v>1</v>
+      </c>
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL27" s="1">
         <v>3</v>
       </c>
       <c r="AM27" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN27" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO27" s="8">
         <v>0</v>
       </c>
       <c r="AP27" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ27" s="5"/>
     </row>
@@ -3185,7 +3223,9 @@
       <c r="U28" s="9">
         <v>0.2</v>
       </c>
-      <c r="V28" s="1"/>
+      <c r="V28" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
@@ -3194,23 +3234,23 @@
       <c r="AB28" s="1"/>
       <c r="AC28" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD28" s="1">
         <f t="shared" si="2"/>
-        <v>4.2</v>
+        <v>4.3</v>
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>0.80769230769230771</v>
+        <v>0.69354838709677413</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
@@ -3235,7 +3275,7 @@
       </c>
       <c r="AP28" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ28" s="5"/>
     </row>
@@ -3278,7 +3318,9 @@
       <c r="U29" s="9">
         <v>0</v>
       </c>
-      <c r="V29" s="1"/>
+      <c r="V29" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
@@ -3287,19 +3329,19 @@
       <c r="AB29" s="1"/>
       <c r="AC29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD29" s="1">
         <f t="shared" si="2"/>
-        <v>5.3</v>
+        <v>5.3999999999999995</v>
       </c>
       <c r="AE29" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF29" s="7">
         <f t="shared" si="4"/>
-        <v>1.0192307692307692</v>
+        <v>0.87096774193548376</v>
       </c>
       <c r="AG29" s="4">
         <f t="shared" si="5"/>
@@ -3348,7 +3390,7 @@
         <v>1.5</v>
       </c>
       <c r="G30" s="1">
-        <v>0.35</v>
+        <v>0.65</v>
       </c>
       <c r="H30" s="1">
         <v>0.6</v>
@@ -3366,7 +3408,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1">
         <f t="shared" si="0"/>
-        <v>4.45</v>
+        <v>4.75</v>
       </c>
       <c r="U30" s="9">
         <v>0</v>
@@ -3384,19 +3426,19 @@
       </c>
       <c r="AD30" s="1">
         <f t="shared" si="2"/>
-        <v>4.45</v>
+        <v>4.75</v>
       </c>
       <c r="AE30" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF30" s="7">
         <f t="shared" si="4"/>
-        <v>0.85576923076923073</v>
+        <v>0.7661290322580645</v>
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
@@ -3421,7 +3463,7 @@
       </c>
       <c r="AP30" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ30" s="5"/>
     </row>
@@ -3446,7 +3488,9 @@
       <c r="H31" s="1">
         <v>1.5</v>
       </c>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3459,12 +3503,14 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="U31" s="9">
         <v>0.2</v>
       </c>
-      <c r="V31" s="1"/>
+      <c r="V31" s="1">
+        <v>0.1</v>
+      </c>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
@@ -3473,19 +3519,19 @@
       <c r="AB31" s="1"/>
       <c r="AC31" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD31" s="1">
         <f t="shared" si="2"/>
-        <v>6.7</v>
+        <v>7.8</v>
       </c>
       <c r="AE31" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF31" s="7">
         <f t="shared" si="4"/>
-        <v>1.2884615384615385</v>
+        <v>1.2580645161290323</v>
       </c>
       <c r="AG31" s="4">
         <f t="shared" si="5"/>
@@ -3574,11 +3620,11 @@
       </c>
       <c r="AE32" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF32" s="7">
         <f t="shared" si="4"/>
-        <v>1.1057692307692308</v>
+        <v>0.92741935483870963</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="5"/>
@@ -3665,11 +3711,11 @@
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>0.96153846153846145</v>
+        <v>0.80645161290322576</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
@@ -3723,7 +3769,9 @@
       <c r="H34" s="1">
         <v>1.5</v>
       </c>
-      <c r="I34" s="1"/>
+      <c r="I34" s="1">
+        <v>1.5</v>
+      </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -3736,7 +3784,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="U34" s="9">
         <v>0</v>
@@ -3754,15 +3802,15 @@
       </c>
       <c r="AD34" s="1">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.2903225806451613</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>
@@ -3816,7 +3864,9 @@
       <c r="H35" s="1">
         <v>1</v>
       </c>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -3829,7 +3879,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1">
         <f t="shared" ref="T35" si="10">SUM(C35:S35)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U35" s="1">
         <v>0.2</v>
@@ -3847,11 +3897,11 @@
       </c>
       <c r="AD35" s="1">
         <f t="shared" ref="AD35" si="12">T35+AC35</f>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AE35" s="4">
         <f>AD35</f>
-        <v>5.2</v>
+        <v>6.2</v>
       </c>
       <c r="AF35" s="7">
         <f t="shared" ref="AF35" si="13">(AD35/AE35)</f>

</xml_diff>

<commit_message>
Update achievement. Add links.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D36F41-0018-4A40-84FD-A960F68F543D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C891A1-382D-44E0-92FB-65043AAA5065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -602,12 +602,14 @@
     <col min="4" max="4" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.8984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="3.296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="13" max="19" width="4.296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="28" width="4.296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="4.296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="4.296875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="3.8984375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="5.3984375" bestFit="1" customWidth="1"/>
@@ -795,26 +797,28 @@
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
+      <c r="X2" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1">
         <f t="shared" ref="AC2:AC34" si="1">SUM(U2:AB2)</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD2" s="1">
         <f t="shared" ref="AD2:AD34" si="2">T2+AC2</f>
-        <v>4.9499999999999993</v>
+        <v>5.05</v>
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.79838709677419339</v>
+        <v>0.64743589743589747</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
@@ -866,7 +870,9 @@
         <v>0.65</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1">
+        <v>0.1</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -879,33 +885,35 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1">
         <f t="shared" si="0"/>
-        <v>4.6500000000000004</v>
+        <v>4.75</v>
       </c>
       <c r="U3" s="1">
         <v>0</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
+      <c r="X3" s="1">
+        <v>0.05</v>
+      </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AD3" s="1">
         <f t="shared" si="2"/>
-        <v>4.6500000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
@@ -979,30 +987,32 @@
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
+      <c r="X4" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD4" s="1">
         <f t="shared" si="2"/>
-        <v>4.25</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.68548387096774188</v>
+        <v>0.55769230769230771</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1027,7 +1037,7 @@
       </c>
       <c r="AP4" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ4" s="5"/>
     </row>
@@ -1050,7 +1060,9 @@
       <c r="H5" s="1">
         <v>0.6</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1063,7 +1075,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1">
         <f t="shared" si="0"/>
-        <v>4.0999999999999996</v>
+        <v>4.6999999999999993</v>
       </c>
       <c r="U5" s="9">
         <v>0.1</v>
@@ -1081,15 +1093,15 @@
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="2"/>
-        <v>4.1999999999999993</v>
+        <v>4.7999999999999989</v>
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="4"/>
-        <v>0.67741935483870952</v>
+        <v>0.61538461538461531</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="5"/>
@@ -1176,11 +1188,11 @@
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" si="4"/>
-        <v>0.58870967741935476</v>
+        <v>0.46794871794871795</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="5"/>
@@ -1237,7 +1249,9 @@
       <c r="I7" s="1">
         <v>0.6</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>0.6</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1249,33 +1263,35 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>7.1</v>
+        <v>7.6999999999999993</v>
       </c>
       <c r="U7" s="9">
         <v>0</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
+      <c r="X7" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="2"/>
-        <v>7.1</v>
+        <v>7.7999999999999989</v>
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>1.1451612903225805</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
@@ -1351,30 +1367,32 @@
       </c>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
+      <c r="X8" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="2"/>
-        <v>5.85</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="AE8" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF8" s="7">
         <f t="shared" si="4"/>
-        <v>0.94354838709677413</v>
+        <v>0.76282051282051277</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
@@ -1399,7 +1417,7 @@
       </c>
       <c r="AP8" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ8" s="5"/>
     </row>
@@ -1442,26 +1460,28 @@
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
+      <c r="X9" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="2"/>
-        <v>4.8500000000000005</v>
+        <v>4.95</v>
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>0.78225806451612911</v>
+        <v>0.63461538461538469</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
@@ -1515,8 +1535,12 @@
       <c r="H10" s="1">
         <v>1.5</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.6</v>
+      </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1528,33 +1552,35 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>8.1</v>
       </c>
       <c r="U10" s="9">
         <v>0.1</v>
       </c>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
+      <c r="X10" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD10" s="1">
         <f t="shared" si="2"/>
-        <v>6.6</v>
+        <v>8.2999999999999989</v>
       </c>
       <c r="AE10" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF10" s="7">
         <f t="shared" si="4"/>
-        <v>1.064516129032258</v>
+        <v>1.0641025641025641</v>
       </c>
       <c r="AG10" s="4">
         <f t="shared" si="5"/>
@@ -1608,7 +1634,9 @@
       <c r="H11" s="1">
         <v>1.5</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <v>0.05</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1621,7 +1649,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1">
         <f t="shared" si="0"/>
-        <v>6.5</v>
+        <v>6.55</v>
       </c>
       <c r="U11" s="9">
         <v>0</v>
@@ -1639,15 +1667,15 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>6.55</v>
       </c>
       <c r="AE11" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF11" s="7">
         <f t="shared" si="4"/>
-        <v>1.0483870967741935</v>
+        <v>0.83974358974358976</v>
       </c>
       <c r="AG11" s="4">
         <f t="shared" si="5"/>
@@ -1701,7 +1729,9 @@
       <c r="H12" s="1">
         <v>0.8</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <v>0.5</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1714,7 +1744,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="U12" s="9">
         <v>0</v>
@@ -1723,26 +1753,28 @@
         <v>0.1</v>
       </c>
       <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
+      <c r="X12" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="2"/>
-        <v>5.8999999999999995</v>
+        <v>6.5</v>
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>0.95161290322580638</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
@@ -1818,26 +1850,28 @@
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
+      <c r="X13" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
+        <v>4.9499999999999993</v>
       </c>
       <c r="AE13" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF13" s="7">
         <f t="shared" si="4"/>
-        <v>0.782258064516129</v>
+        <v>0.63461538461538458</v>
       </c>
       <c r="AG13" s="4">
         <f t="shared" si="5"/>
@@ -1913,26 +1947,28 @@
         <v>0.1</v>
       </c>
       <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
+      <c r="X14" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="2"/>
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="AE14" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF14" s="7">
         <f t="shared" si="4"/>
-        <v>1.0161290322580645</v>
+        <v>0.8205128205128206</v>
       </c>
       <c r="AG14" s="4">
         <f t="shared" si="5"/>
@@ -1983,9 +2019,13 @@
       <c r="G15" s="1">
         <v>0.65</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>0.4</v>
+      </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="1">
+        <v>0.3</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1997,7 +2037,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1">
         <f t="shared" si="0"/>
-        <v>4.1500000000000004</v>
+        <v>4.8500000000000005</v>
       </c>
       <c r="U15" s="9">
         <v>0</v>
@@ -2015,15 +2055,15 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="2"/>
-        <v>4.1500000000000004</v>
+        <v>4.8500000000000005</v>
       </c>
       <c r="AE15" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF15" s="7">
         <f t="shared" si="4"/>
-        <v>0.66935483870967749</v>
+        <v>0.62179487179487192</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="5"/>
@@ -2078,9 +2118,11 @@
         <v>1</v>
       </c>
       <c r="I16" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="J16" s="1">
         <v>0.6</v>
       </c>
-      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2092,33 +2134,35 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1">
         <f t="shared" si="0"/>
-        <v>6.25</v>
+        <v>7.05</v>
       </c>
       <c r="U16" s="9">
         <v>0</v>
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
+      <c r="X16" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD16" s="1">
         <f t="shared" si="2"/>
-        <v>6.25</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="AE16" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF16" s="7">
         <f t="shared" si="4"/>
-        <v>1.0080645161290323</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="AG16" s="4">
         <f t="shared" si="5"/>
@@ -2170,7 +2214,9 @@
         <v>0.65</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>0.6</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2183,33 +2229,35 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1">
         <f t="shared" si="0"/>
-        <v>4.1500000000000004</v>
+        <v>4.75</v>
       </c>
       <c r="U17" s="9">
         <v>0.1</v>
       </c>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
+      <c r="X17" s="1">
+        <v>0.1</v>
+      </c>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="2"/>
-        <v>4.25</v>
+        <v>4.95</v>
       </c>
       <c r="AE17" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF17" s="7">
         <f t="shared" si="4"/>
-        <v>0.68548387096774188</v>
+        <v>0.63461538461538469</v>
       </c>
       <c r="AG17" s="4">
         <f t="shared" si="5"/>
@@ -2296,15 +2344,15 @@
       </c>
       <c r="AE18" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF18" s="7">
         <f t="shared" si="4"/>
-        <v>0.75</v>
+        <v>0.59615384615384626</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2329,7 +2377,7 @@
       </c>
       <c r="AP18" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ18" s="5"/>
     </row>
@@ -2355,7 +2403,7 @@
         <v>0.6</v>
       </c>
       <c r="I19" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -2369,7 +2417,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1">
         <f t="shared" si="0"/>
-        <v>6.1999999999999993</v>
+        <v>6.6</v>
       </c>
       <c r="U19" s="9">
         <v>0.1</v>
@@ -2378,26 +2426,28 @@
         <v>0.1</v>
       </c>
       <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
+      <c r="X19" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="2"/>
-        <v>6.3999999999999995</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>1.032258064516129</v>
+        <v>0.88461538461538458</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
@@ -2454,9 +2504,13 @@
       <c r="I20" s="1">
         <v>1.5</v>
       </c>
-      <c r="J20" s="1"/>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -2466,7 +2520,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U20" s="9">
         <v>0.1</v>
@@ -2474,56 +2528,62 @@
       <c r="V20" s="1">
         <v>0.1</v>
       </c>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
+      <c r="W20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="X20" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="2"/>
-        <v>8.1999999999999993</v>
+        <v>10.4</v>
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>1.3225806451612903</v>
+        <v>1.3333333333333335</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="AH20" s="1"/>
+      <c r="AH20" s="1">
+        <v>1</v>
+      </c>
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL20" s="1">
         <v>3</v>
       </c>
       <c r="AM20" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN20" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO20" s="8">
         <v>0</v>
       </c>
       <c r="AP20" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ20" s="5"/>
     </row>
@@ -2581,11 +2641,11 @@
       </c>
       <c r="AE21" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF21" s="7">
         <f t="shared" si="4"/>
-        <v>0.58870967741935476</v>
+        <v>0.46794871794871795</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="5"/>
@@ -2640,7 +2700,7 @@
         <v>1.5</v>
       </c>
       <c r="I22" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2654,7 +2714,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1">
         <f t="shared" si="0"/>
-        <v>7.1</v>
+        <v>7.5</v>
       </c>
       <c r="U22" s="1">
         <v>0.1</v>
@@ -2663,26 +2723,28 @@
         <v>0.1</v>
       </c>
       <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
+      <c r="X22" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="2"/>
-        <v>7.3</v>
+        <v>7.8</v>
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>1.1774193548387095</v>
+        <v>1</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
@@ -2767,11 +2829,11 @@
       </c>
       <c r="AE23" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF23" s="7">
         <f t="shared" si="4"/>
-        <v>0.56451612903225801</v>
+        <v>0.44871794871794873</v>
       </c>
       <c r="AG23" s="8">
         <f t="shared" si="5"/>
@@ -2828,7 +2890,9 @@
       <c r="I24" s="1">
         <v>1.5</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2840,33 +2904,35 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="U24" s="9">
         <v>0</v>
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
+      <c r="X24" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD24" s="1">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>8.6</v>
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>1.2096774193548387</v>
+        <v>1.1025641025641026</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
@@ -2955,15 +3021,15 @@
       </c>
       <c r="AE25" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF25" s="7">
         <f t="shared" si="4"/>
-        <v>0.84677419354838712</v>
+        <v>0.67307692307692313</v>
       </c>
       <c r="AG25" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
@@ -2988,7 +3054,7 @@
       </c>
       <c r="AP25" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ25" s="5"/>
     </row>
@@ -3014,9 +3080,11 @@
         <v>1.5</v>
       </c>
       <c r="I26" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="J26" s="1">
         <v>1</v>
       </c>
-      <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -3028,7 +3096,7 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>9</v>
       </c>
       <c r="U26" s="9">
         <v>0</v>
@@ -3037,26 +3105,28 @@
         <v>0.1</v>
       </c>
       <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
+      <c r="X26" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
       <c r="AC26" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD26" s="1">
         <f t="shared" si="2"/>
-        <v>7.6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AE26" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF26" s="7">
         <f t="shared" si="4"/>
-        <v>1.225806451612903</v>
+        <v>1.1794871794871795</v>
       </c>
       <c r="AG26" s="4">
         <f t="shared" si="5"/>
@@ -3113,9 +3183,13 @@
       <c r="I27" s="1">
         <v>1.5</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
       <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -3125,7 +3199,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U27" s="9">
         <v>0.2</v>
@@ -3133,27 +3207,31 @@
       <c r="V27" s="1">
         <v>0.2</v>
       </c>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
+      <c r="W27" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="X27" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="2"/>
-        <v>8.4</v>
+        <v>10.7</v>
       </c>
       <c r="AE27" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF27" s="7">
         <f t="shared" si="4"/>
-        <v>1.3548387096774195</v>
+        <v>1.3717948717948718</v>
       </c>
       <c r="AG27" s="4">
         <f t="shared" si="5"/>
@@ -3206,7 +3284,9 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="J28" s="1">
+        <v>0.6</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -3218,7 +3298,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="U28" s="9">
         <v>0.2</v>
@@ -3227,26 +3307,28 @@
         <v>0.1</v>
       </c>
       <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
+      <c r="X28" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="AD28" s="1">
         <f t="shared" si="2"/>
-        <v>4.3</v>
+        <v>5</v>
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>0.69354838709677413</v>
+        <v>0.64102564102564108</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
@@ -3300,8 +3382,12 @@
       <c r="H29" s="1">
         <v>1</v>
       </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="I29" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.1</v>
+      </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -3313,7 +3399,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1">
         <f t="shared" si="0"/>
-        <v>5.3</v>
+        <v>5.9999999999999991</v>
       </c>
       <c r="U29" s="9">
         <v>0</v>
@@ -3333,19 +3419,19 @@
       </c>
       <c r="AD29" s="1">
         <f t="shared" si="2"/>
-        <v>5.3999999999999995</v>
+        <v>6.0999999999999988</v>
       </c>
       <c r="AE29" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF29" s="7">
         <f t="shared" si="4"/>
-        <v>0.87096774193548376</v>
+        <v>0.78205128205128194</v>
       </c>
       <c r="AG29" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -3370,7 +3456,7 @@
       </c>
       <c r="AP29" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ29" s="5"/>
     </row>
@@ -3430,11 +3516,11 @@
       </c>
       <c r="AE30" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF30" s="7">
         <f t="shared" si="4"/>
-        <v>0.7661290322580645</v>
+        <v>0.60897435897435903</v>
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="5"/>
@@ -3491,7 +3577,9 @@
       <c r="I31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1"/>
+      <c r="J31" s="1">
+        <v>0.6</v>
+      </c>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -3503,7 +3591,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>8.1</v>
       </c>
       <c r="U31" s="9">
         <v>0.2</v>
@@ -3512,26 +3600,28 @@
         <v>0.1</v>
       </c>
       <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
+      <c r="X31" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="AD31" s="1">
         <f t="shared" si="2"/>
-        <v>7.8</v>
+        <v>8.6</v>
       </c>
       <c r="AE31" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF31" s="7">
         <f t="shared" si="4"/>
-        <v>1.2580645161290323</v>
+        <v>1.1025641025641026</v>
       </c>
       <c r="AG31" s="4">
         <f t="shared" si="5"/>
@@ -3585,8 +3675,12 @@
       <c r="H32" s="9">
         <v>1</v>
       </c>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
+      <c r="I32" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.1</v>
+      </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
@@ -3598,7 +3692,7 @@
       <c r="S32" s="9"/>
       <c r="T32" s="9">
         <f t="shared" si="0"/>
-        <v>5.65</v>
+        <v>6.05</v>
       </c>
       <c r="U32" s="9">
         <v>0.1</v>
@@ -3616,19 +3710,19 @@
       </c>
       <c r="AD32" s="9">
         <f t="shared" si="2"/>
-        <v>5.75</v>
+        <v>6.1499999999999995</v>
       </c>
       <c r="AE32" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF32" s="7">
         <f t="shared" si="4"/>
-        <v>0.92741935483870963</v>
+        <v>0.78846153846153844</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH32" s="9"/>
       <c r="AI32" s="9"/>
@@ -3653,7 +3747,7 @@
       </c>
       <c r="AP32" s="8">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ32" s="5"/>
     </row>
@@ -3711,15 +3805,15 @@
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>0.80645161290322576</v>
+        <v>0.64102564102564108</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH33" s="9"/>
       <c r="AI33" s="9"/>
@@ -3744,7 +3838,7 @@
       </c>
       <c r="AP33" s="8">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ33" s="5"/>
     </row>
@@ -3772,7 +3866,9 @@
       <c r="I34" s="1">
         <v>1.5</v>
       </c>
-      <c r="J34" s="1"/>
+      <c r="J34" s="1">
+        <v>1</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -3784,33 +3880,35 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U34" s="9">
         <v>0</v>
       </c>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
+      <c r="X34" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD34" s="1">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9.1</v>
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>1.2903225806451613</v>
+        <v>1.1666666666666667</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>
@@ -3867,7 +3965,9 @@
       <c r="I35" s="1">
         <v>1</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3879,29 +3979,35 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1">
         <f t="shared" ref="T35" si="10">SUM(C35:S35)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U35" s="1">
         <v>0.2</v>
       </c>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
+      <c r="V35" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="W35" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="X35" s="1">
+        <v>0.2</v>
+      </c>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1">
         <f t="shared" ref="AC35" si="11">SUM(U35:AB35)</f>
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="AD35" s="1">
         <f t="shared" ref="AD35" si="12">T35+AC35</f>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AE35" s="4">
         <f>AD35</f>
-        <v>6.2</v>
+        <v>7.8</v>
       </c>
       <c r="AF35" s="7">
         <f t="shared" ref="AF35" si="13">(AD35/AE35)</f>

</xml_diff>

<commit_message>
Update achievement. Add solutions-6,7.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C891A1-382D-44E0-92FB-65043AAA5065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937A7124-4223-43CB-ABB4-FE1038A6FD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -591,7 +591,7 @@
   <dimension ref="A1:AQ230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -602,8 +602,7 @@
     <col min="4" max="4" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="13" max="19" width="4.296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.8984375" bestFit="1" customWidth="1"/>
@@ -778,7 +777,9 @@
       <c r="I2" s="1">
         <v>0.1</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1">
+        <v>0.6</v>
+      </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -790,7 +791,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f t="shared" ref="T2:T34" si="0">SUM(C2:S2)</f>
-        <v>4.8499999999999996</v>
+        <v>5.4499999999999993</v>
       </c>
       <c r="U2" s="9">
         <v>0.1</v>
@@ -810,19 +811,19 @@
       </c>
       <c r="AD2" s="1">
         <f t="shared" ref="AD2:AD34" si="2">T2+AC2</f>
-        <v>5.05</v>
+        <v>5.6499999999999995</v>
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.64743589743589747</v>
+        <v>0.57653061224489788</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
@@ -847,7 +848,7 @@
       </c>
       <c r="AP2" s="4">
         <f t="shared" ref="AP2:AP34" si="9">(AG2+AN2+AO2)/3</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ2" s="5"/>
     </row>
@@ -909,15 +910,15 @@
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>0.61538461538461542</v>
+        <v>0.48979591836734687</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -942,7 +943,7 @@
       </c>
       <c r="AP3" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ3" s="5"/>
     </row>
@@ -1004,11 +1005,11 @@
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.55769230769230771</v>
+        <v>0.4438775510204081</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
@@ -1097,15 +1098,15 @@
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="4"/>
-        <v>0.61538461538461531</v>
+        <v>0.48979591836734682</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -1130,7 +1131,7 @@
       </c>
       <c r="AP5" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ5" s="5"/>
     </row>
@@ -1154,7 +1155,9 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1">
+        <v>0.1</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1166,7 +1169,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>3.75</v>
       </c>
       <c r="U6" s="9">
         <v>0</v>
@@ -1184,19 +1187,19 @@
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="2"/>
-        <v>3.65</v>
+        <v>3.75</v>
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" si="4"/>
-        <v>0.46794871794871795</v>
+        <v>0.38265306122448978</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
@@ -1221,7 +1224,7 @@
       </c>
       <c r="AP6" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AQ6" s="5"/>
     </row>
@@ -1287,15 +1290,15 @@
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>0.99999999999999989</v>
+        <v>0.79591836734693866</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
@@ -1320,7 +1323,7 @@
       </c>
       <c r="AP7" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ7" s="5"/>
     </row>
@@ -1384,11 +1387,11 @@
       </c>
       <c r="AE8" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF8" s="7">
         <f t="shared" si="4"/>
-        <v>0.76282051282051277</v>
+        <v>0.60714285714285698</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="5"/>
@@ -1477,15 +1480,15 @@
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>0.63461538461538469</v>
+        <v>0.50510204081632648</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
@@ -1510,7 +1513,7 @@
       </c>
       <c r="AP9" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ9" s="5"/>
     </row>
@@ -1576,11 +1579,11 @@
       </c>
       <c r="AE10" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF10" s="7">
         <f t="shared" si="4"/>
-        <v>1.0641025641025641</v>
+        <v>0.84693877551020391</v>
       </c>
       <c r="AG10" s="4">
         <f t="shared" si="5"/>
@@ -1671,15 +1674,15 @@
       </c>
       <c r="AE11" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF11" s="7">
         <f t="shared" si="4"/>
-        <v>0.83974358974358976</v>
+        <v>0.66836734693877542</v>
       </c>
       <c r="AG11" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
@@ -1704,7 +1707,7 @@
       </c>
       <c r="AP11" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ11" s="5"/>
     </row>
@@ -1770,15 +1773,15 @@
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>0.83333333333333337</v>
+        <v>0.66326530612244894</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
@@ -1803,7 +1806,7 @@
       </c>
       <c r="AP12" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ12" s="5"/>
     </row>
@@ -1831,7 +1834,9 @@
       <c r="I13" s="1">
         <v>0.1</v>
       </c>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1">
+        <v>0.35</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1843,7 +1848,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>4.8499999999999996</v>
+        <v>5.1999999999999993</v>
       </c>
       <c r="U13" s="9">
         <v>0</v>
@@ -1863,44 +1868,46 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="2"/>
-        <v>4.9499999999999993</v>
+        <v>5.2999999999999989</v>
       </c>
       <c r="AE13" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF13" s="7">
         <f t="shared" si="4"/>
-        <v>0.63461538461538458</v>
+        <v>0.54081632653061207</v>
       </c>
       <c r="AG13" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AH13" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>1</v>
+      </c>
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL13" s="1">
         <v>3</v>
       </c>
       <c r="AM13" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN13" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO13" s="8">
         <v>0</v>
       </c>
       <c r="AP13" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="AQ13" s="5"/>
     </row>
@@ -1926,7 +1933,9 @@
       <c r="I14" s="1">
         <v>1</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1">
+        <v>1</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1938,7 +1947,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U14" s="9">
         <v>0.2</v>
@@ -1960,19 +1969,19 @@
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="2"/>
-        <v>6.4</v>
+        <v>7.4</v>
       </c>
       <c r="AE14" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF14" s="7">
         <f t="shared" si="4"/>
-        <v>0.8205128205128206</v>
+        <v>0.75510204081632648</v>
       </c>
       <c r="AG14" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
@@ -1997,7 +2006,7 @@
       </c>
       <c r="AP14" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ14" s="5"/>
     </row>
@@ -2059,15 +2068,15 @@
       </c>
       <c r="AE15" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF15" s="7">
         <f t="shared" si="4"/>
-        <v>0.62179487179487192</v>
+        <v>0.49489795918367346</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
@@ -2092,7 +2101,7 @@
       </c>
       <c r="AP15" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ15" s="5"/>
     </row>
@@ -2158,15 +2167,15 @@
       </c>
       <c r="AE16" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF16" s="7">
         <f t="shared" si="4"/>
-        <v>0.91666666666666663</v>
+        <v>0.72959183673469374</v>
       </c>
       <c r="AG16" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -2191,7 +2200,7 @@
       </c>
       <c r="AP16" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ16" s="5"/>
     </row>
@@ -2253,15 +2262,15 @@
       </c>
       <c r="AE17" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF17" s="7">
         <f t="shared" si="4"/>
-        <v>0.63461538461538469</v>
+        <v>0.50510204081632648</v>
       </c>
       <c r="AG17" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
@@ -2286,7 +2295,7 @@
       </c>
       <c r="AP17" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ17" s="5"/>
     </row>
@@ -2344,11 +2353,11 @@
       </c>
       <c r="AE18" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF18" s="7">
         <f t="shared" si="4"/>
-        <v>0.59615384615384626</v>
+        <v>0.47448979591836737</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" si="5"/>
@@ -2443,15 +2452,15 @@
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>0.88461538461538458</v>
+        <v>0.70408163265306112</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2476,7 +2485,7 @@
       </c>
       <c r="AP19" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ19" s="5"/>
     </row>
@@ -2548,11 +2557,11 @@
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>1.3333333333333335</v>
+        <v>1.0612244897959184</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
@@ -2607,7 +2616,9 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
+      <c r="J21" s="1">
+        <v>0.1</v>
+      </c>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -2619,7 +2630,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1">
         <f t="shared" si="0"/>
-        <v>3.65</v>
+        <v>3.75</v>
       </c>
       <c r="U21" s="9">
         <v>0</v>
@@ -2637,19 +2648,19 @@
       </c>
       <c r="AD21" s="1">
         <f t="shared" si="2"/>
-        <v>3.65</v>
+        <v>3.75</v>
       </c>
       <c r="AE21" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF21" s="7">
         <f t="shared" si="4"/>
-        <v>0.46794871794871795</v>
+        <v>0.38265306122448978</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
@@ -2674,7 +2685,7 @@
       </c>
       <c r="AP21" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AQ21" s="5"/>
     </row>
@@ -2702,7 +2713,9 @@
       <c r="I22" s="1">
         <v>1</v>
       </c>
-      <c r="J22" s="1"/>
+      <c r="J22" s="1">
+        <v>0.6</v>
+      </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -2714,7 +2727,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1">
         <f t="shared" si="0"/>
-        <v>7.5</v>
+        <v>8.1</v>
       </c>
       <c r="U22" s="1">
         <v>0.1</v>
@@ -2736,15 +2749,15 @@
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="2"/>
-        <v>7.8</v>
+        <v>8.4</v>
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
@@ -2829,15 +2842,15 @@
       </c>
       <c r="AE23" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF23" s="7">
         <f t="shared" si="4"/>
-        <v>0.44871794871794873</v>
+        <v>0.3571428571428571</v>
       </c>
       <c r="AG23" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH23" s="9"/>
       <c r="AI23" s="9"/>
@@ -2862,7 +2875,7 @@
       </c>
       <c r="AP23" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AQ23" s="5"/>
     </row>
@@ -2928,11 +2941,11 @@
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>1.1025641025641026</v>
+        <v>0.87755102040816313</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
@@ -3021,15 +3034,15 @@
       </c>
       <c r="AE25" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF25" s="7">
         <f t="shared" si="4"/>
-        <v>0.67307692307692313</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="AG25" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
@@ -3054,7 +3067,7 @@
       </c>
       <c r="AP25" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ25" s="5"/>
     </row>
@@ -3122,11 +3135,11 @@
       </c>
       <c r="AE26" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF26" s="7">
         <f t="shared" si="4"/>
-        <v>1.1794871794871795</v>
+        <v>0.93877551020408145</v>
       </c>
       <c r="AG26" s="4">
         <f t="shared" si="5"/>
@@ -3227,11 +3240,11 @@
       </c>
       <c r="AE27" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF27" s="7">
         <f t="shared" si="4"/>
-        <v>1.3717948717948718</v>
+        <v>1.0918367346938773</v>
       </c>
       <c r="AG27" s="4">
         <f t="shared" si="5"/>
@@ -3324,15 +3337,15 @@
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>0.64102564102564108</v>
+        <v>0.51020408163265307</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
@@ -3357,7 +3370,7 @@
       </c>
       <c r="AP28" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ28" s="5"/>
     </row>
@@ -3386,7 +3399,7 @@
         <v>0.6</v>
       </c>
       <c r="J29" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -3399,7 +3412,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1">
         <f t="shared" si="0"/>
-        <v>5.9999999999999991</v>
+        <v>6.1999999999999993</v>
       </c>
       <c r="U29" s="9">
         <v>0</v>
@@ -3419,15 +3432,15 @@
       </c>
       <c r="AD29" s="1">
         <f t="shared" si="2"/>
-        <v>6.0999999999999988</v>
+        <v>6.2999999999999989</v>
       </c>
       <c r="AE29" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF29" s="7">
         <f t="shared" si="4"/>
-        <v>0.78205128205128194</v>
+        <v>0.64285714285714268</v>
       </c>
       <c r="AG29" s="4">
         <f t="shared" si="5"/>
@@ -3516,15 +3529,15 @@
       </c>
       <c r="AE30" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF30" s="7">
         <f t="shared" si="4"/>
-        <v>0.60897435897435903</v>
+        <v>0.48469387755102039</v>
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
@@ -3549,7 +3562,7 @@
       </c>
       <c r="AP30" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ30" s="5"/>
     </row>
@@ -3617,11 +3630,11 @@
       </c>
       <c r="AE31" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF31" s="7">
         <f t="shared" si="4"/>
-        <v>1.1025641025641026</v>
+        <v>0.87755102040816313</v>
       </c>
       <c r="AG31" s="4">
         <f t="shared" si="5"/>
@@ -3714,11 +3727,11 @@
       </c>
       <c r="AE32" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF32" s="7">
         <f t="shared" si="4"/>
-        <v>0.78846153846153844</v>
+        <v>0.62755102040816313</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="5"/>
@@ -3805,15 +3818,15 @@
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>0.64102564102564108</v>
+        <v>0.51020408163265307</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH33" s="9"/>
       <c r="AI33" s="9"/>
@@ -3838,7 +3851,7 @@
       </c>
       <c r="AP33" s="8">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ33" s="5"/>
     </row>
@@ -3904,11 +3917,11 @@
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>1.1666666666666667</v>
+        <v>0.92857142857142849</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>
@@ -3951,19 +3964,19 @@
         <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="F35" s="9">
+        <v>1.5</v>
       </c>
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="H35" s="1">
-        <v>1</v>
-      </c>
-      <c r="I35" s="1">
-        <v>1</v>
+      <c r="H35" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="I35" s="9">
+        <v>1.5</v>
       </c>
       <c r="J35" s="1">
         <v>1</v>
@@ -3979,7 +3992,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1">
         <f t="shared" ref="T35" si="10">SUM(C35:S35)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U35" s="1">
         <v>0.2</v>
@@ -4003,11 +4016,11 @@
       </c>
       <c r="AD35" s="1">
         <f t="shared" ref="AD35" si="12">T35+AC35</f>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AE35" s="4">
         <f>AD35</f>
-        <v>7.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AF35" s="7">
         <f t="shared" ref="AF35" si="13">(AD35/AE35)</f>

</xml_diff>

<commit_message>
Update achievement. Update classes 10.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937A7124-4223-43CB-ABB4-FE1038A6FD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5D1D5-CF7D-42B9-BE3D-3C713BEBDEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,8 @@
     <col min="5" max="5" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="4.8984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="3.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.8984375" bestFit="1" customWidth="1"/>
     <col min="13" max="19" width="4.296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="4.296875" bestFit="1" customWidth="1"/>
@@ -614,7 +615,8 @@
     <col min="31" max="31" width="5.3984375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8.19921875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="3.296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="6" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="5.3984375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="2.69921875" bestFit="1" customWidth="1"/>
@@ -815,29 +817,31 @@
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.57653061224489788</v>
+        <v>0.52314814814814803</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
         <v>3</v>
       </c>
-      <c r="AH2" s="1"/>
+      <c r="AH2" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1">
         <f t="shared" ref="AK2:AK34" si="6">SUM(AH2:AJ2)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL2" s="1">
         <v>3</v>
       </c>
       <c r="AM2" s="4">
         <f t="shared" ref="AM2:AM34" si="7">(AK2/AL2)*100</f>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN2" s="4">
         <f t="shared" ref="AN2:AN34" si="8">MAX(IF(AM2&gt;=20,2,0),IF(AM2&gt;=40,3,0),IF(AM2&gt;=60,4,0),IF(AM2&gt;=80,5,0))</f>
@@ -910,11 +914,11 @@
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>0.48979591836734687</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
@@ -1005,29 +1009,31 @@
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.4438775510204081</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="AH4" s="1"/>
+      <c r="AH4" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL4" s="1">
         <v>3</v>
       </c>
       <c r="AM4" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN4" s="4">
         <f t="shared" si="8"/>
@@ -1098,11 +1104,11 @@
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="4"/>
-        <v>0.48979591836734682</v>
+        <v>0.44444444444444431</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="5"/>
@@ -1191,29 +1197,31 @@
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" si="4"/>
-        <v>0.38265306122448978</v>
+        <v>0.34722222222222221</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="AH6" s="1"/>
+      <c r="AH6" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL6" s="1">
         <v>3</v>
       </c>
       <c r="AM6" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN6" s="4">
         <f t="shared" si="8"/>
@@ -1290,40 +1298,42 @@
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>0.79591836734693866</v>
+        <v>0.7222222222222221</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AH7" s="1"/>
+      <c r="AH7" s="1">
+        <v>1</v>
+      </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL7" s="1">
         <v>3</v>
       </c>
       <c r="AM7" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN7" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO7" s="8">
         <v>0</v>
       </c>
       <c r="AP7" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>2</v>
       </c>
       <c r="AQ7" s="5"/>
     </row>
@@ -1387,29 +1397,31 @@
       </c>
       <c r="AE8" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF8" s="7">
         <f t="shared" si="4"/>
-        <v>0.60714285714285698</v>
+        <v>0.55092592592592582</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AH8" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL8" s="1">
         <v>3</v>
       </c>
       <c r="AM8" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN8" s="4">
         <f t="shared" si="8"/>
@@ -1420,7 +1432,7 @@
       </c>
       <c r="AP8" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="5"/>
     </row>
@@ -1480,11 +1492,11 @@
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>0.50510204081632648</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
@@ -1579,40 +1591,42 @@
       </c>
       <c r="AE10" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF10" s="7">
         <f t="shared" si="4"/>
-        <v>0.84693877551020391</v>
+        <v>0.76851851851851838</v>
       </c>
       <c r="AG10" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AH10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>1</v>
+      </c>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL10" s="1">
         <v>3</v>
       </c>
       <c r="AM10" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN10" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO10" s="8">
         <v>0</v>
       </c>
       <c r="AP10" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
       <c r="AQ10" s="5"/>
     </row>
@@ -1674,29 +1688,31 @@
       </c>
       <c r="AE11" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF11" s="7">
         <f t="shared" si="4"/>
-        <v>0.66836734693877542</v>
+        <v>0.6064814814814814</v>
       </c>
       <c r="AG11" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AH11" s="1"/>
+      <c r="AH11" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL11" s="1">
         <v>3</v>
       </c>
       <c r="AM11" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN11" s="4">
         <f t="shared" si="8"/>
@@ -1773,29 +1789,31 @@
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>0.66326530612244894</v>
+        <v>0.60185185185185186</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AH12" s="1"/>
+      <c r="AH12" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL12" s="1">
         <v>3</v>
       </c>
       <c r="AM12" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN12" s="4">
         <f t="shared" si="8"/>
@@ -1838,7 +1856,9 @@
         <v>0.35</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="1">
+        <v>0.6</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1848,7 +1868,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>5.1999999999999993</v>
+        <v>5.7999999999999989</v>
       </c>
       <c r="U13" s="9">
         <v>0</v>
@@ -1868,15 +1888,15 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="2"/>
-        <v>5.2999999999999989</v>
+        <v>5.8999999999999986</v>
       </c>
       <c r="AE13" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF13" s="7">
         <f t="shared" si="4"/>
-        <v>0.54081632653061207</v>
+        <v>0.54629629629629617</v>
       </c>
       <c r="AG13" s="4">
         <f t="shared" si="5"/>
@@ -1973,40 +1993,42 @@
       </c>
       <c r="AE14" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF14" s="7">
         <f t="shared" si="4"/>
-        <v>0.75510204081632648</v>
+        <v>0.68518518518518512</v>
       </c>
       <c r="AG14" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AH14" s="1"/>
+      <c r="AH14" s="1">
+        <v>1</v>
+      </c>
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="1">
         <v>3</v>
       </c>
       <c r="AM14" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN14" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO14" s="8">
         <v>0</v>
       </c>
       <c r="AP14" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>2</v>
       </c>
       <c r="AQ14" s="5"/>
     </row>
@@ -2068,29 +2090,31 @@
       </c>
       <c r="AE15" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF15" s="7">
         <f t="shared" si="4"/>
-        <v>0.49489795918367346</v>
+        <v>0.44907407407407407</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="AH15" s="1"/>
+      <c r="AH15" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL15" s="1">
         <v>3</v>
       </c>
       <c r="AM15" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN15" s="4">
         <f t="shared" si="8"/>
@@ -2167,29 +2191,31 @@
       </c>
       <c r="AE16" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF16" s="7">
         <f t="shared" si="4"/>
-        <v>0.72959183673469374</v>
+        <v>0.66203703703703698</v>
       </c>
       <c r="AG16" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AH16" s="1"/>
+      <c r="AH16" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL16" s="1">
         <v>3</v>
       </c>
       <c r="AM16" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN16" s="4">
         <f t="shared" si="8"/>
@@ -2262,29 +2288,31 @@
       </c>
       <c r="AE17" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF17" s="7">
         <f t="shared" si="4"/>
-        <v>0.50510204081632648</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="AG17" s="4">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="AH17" s="1"/>
+      <c r="AH17" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL17" s="1">
         <v>3</v>
       </c>
       <c r="AM17" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN17" s="4">
         <f t="shared" si="8"/>
@@ -2353,29 +2381,31 @@
       </c>
       <c r="AE18" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF18" s="7">
         <f t="shared" si="4"/>
-        <v>0.47448979591836737</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="AH18" s="1"/>
+      <c r="AH18" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL18" s="1">
         <v>3</v>
       </c>
       <c r="AM18" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN18" s="4">
         <f t="shared" si="8"/>
@@ -2452,29 +2482,31 @@
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>0.70408163265306112</v>
+        <v>0.63888888888888884</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AH19" s="1"/>
+      <c r="AH19" s="1">
+        <v>0.5</v>
+      </c>
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AL19" s="1">
         <v>3</v>
       </c>
       <c r="AM19" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.666666666666664</v>
       </c>
       <c r="AN19" s="4">
         <f t="shared" si="8"/>
@@ -2520,7 +2552,9 @@
       <c r="L20" s="1">
         <v>1</v>
       </c>
-      <c r="M20" s="1"/>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -2529,7 +2563,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U20" s="9">
         <v>0.1</v>
@@ -2553,15 +2587,15 @@
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="2"/>
-        <v>10.4</v>
+        <v>11.4</v>
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>1.0612244897959184</v>
+        <v>1.0555555555555556</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
@@ -2652,11 +2686,11 @@
       </c>
       <c r="AE21" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF21" s="7">
         <f t="shared" si="4"/>
-        <v>0.38265306122448978</v>
+        <v>0.34722222222222221</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="5"/>
@@ -2753,40 +2787,42 @@
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>0.8571428571428571</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AH22" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>1</v>
+      </c>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL22" s="1">
         <v>3</v>
       </c>
       <c r="AM22" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN22" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO22" s="8">
         <v>0</v>
       </c>
       <c r="AP22" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
       <c r="AQ22" s="5"/>
     </row>
@@ -2842,11 +2878,11 @@
       </c>
       <c r="AE23" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF23" s="7">
         <f t="shared" si="4"/>
-        <v>0.3571428571428571</v>
+        <v>0.32407407407407407</v>
       </c>
       <c r="AG23" s="8">
         <f t="shared" si="5"/>
@@ -2941,40 +2977,42 @@
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>0.87755102040816313</v>
+        <v>0.79629629629629617</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AH24" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="AH24" s="1">
+        <v>1</v>
+      </c>
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL24" s="1">
         <v>3</v>
       </c>
       <c r="AM24" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN24" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO24" s="8">
         <v>0</v>
       </c>
       <c r="AP24" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
       <c r="AQ24" s="5"/>
     </row>
@@ -3034,11 +3072,11 @@
       </c>
       <c r="AE25" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF25" s="7">
         <f t="shared" si="4"/>
-        <v>0.5357142857142857</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="AG25" s="4">
         <f t="shared" si="5"/>
@@ -3135,40 +3173,42 @@
       </c>
       <c r="AE26" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF26" s="7">
         <f t="shared" si="4"/>
-        <v>0.93877551020408145</v>
+        <v>0.85185185185185175</v>
       </c>
       <c r="AG26" s="4">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="AH26" s="1"/>
+      <c r="AH26" s="1">
+        <v>1</v>
+      </c>
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL26" s="1">
         <v>3</v>
       </c>
       <c r="AM26" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN26" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO26" s="8">
         <v>0</v>
       </c>
       <c r="AP26" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ26" s="5"/>
     </row>
@@ -3203,7 +3243,9 @@
       <c r="L27" s="1">
         <v>1</v>
       </c>
-      <c r="M27" s="1"/>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -3212,7 +3254,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U27" s="9">
         <v>0.2</v>
@@ -3236,15 +3278,15 @@
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="2"/>
-        <v>10.7</v>
+        <v>11.7</v>
       </c>
       <c r="AE27" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF27" s="7">
         <f t="shared" si="4"/>
-        <v>1.0918367346938773</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="AG27" s="4">
         <f t="shared" si="5"/>
@@ -3337,40 +3379,42 @@
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>0.51020408163265307</v>
+        <v>0.46296296296296291</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="AH28" s="1"/>
+      <c r="AH28" s="1">
+        <v>1</v>
+      </c>
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL28" s="1">
         <v>3</v>
       </c>
       <c r="AM28" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN28" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO28" s="8">
         <v>0</v>
       </c>
       <c r="AP28" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="AQ28" s="5"/>
     </row>
@@ -3436,15 +3480,15 @@
       </c>
       <c r="AE29" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF29" s="7">
         <f t="shared" si="4"/>
-        <v>0.64285714285714268</v>
+        <v>0.58333333333333315</v>
       </c>
       <c r="AG29" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
@@ -3469,7 +3513,7 @@
       </c>
       <c r="AP29" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ29" s="5"/>
     </row>
@@ -3529,11 +3573,11 @@
       </c>
       <c r="AE30" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF30" s="7">
         <f t="shared" si="4"/>
-        <v>0.48469387755102039</v>
+        <v>0.43981481481481477</v>
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="5"/>
@@ -3630,40 +3674,42 @@
       </c>
       <c r="AE31" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF31" s="7">
         <f t="shared" si="4"/>
-        <v>0.87755102040816313</v>
+        <v>0.79629629629629617</v>
       </c>
       <c r="AG31" s="4">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="AH31" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="AH31" s="1">
+        <v>1</v>
+      </c>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL31" s="1">
         <v>3</v>
       </c>
       <c r="AM31" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN31" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO31" s="8">
         <v>0</v>
       </c>
       <c r="AP31" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
       <c r="AQ31" s="5"/>
     </row>
@@ -3727,15 +3773,15 @@
       </c>
       <c r="AE32" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF32" s="7">
         <f t="shared" si="4"/>
-        <v>0.62755102040816313</v>
+        <v>0.56944444444444431</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH32" s="9"/>
       <c r="AI32" s="9"/>
@@ -3760,7 +3806,7 @@
       </c>
       <c r="AP32" s="8">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ32" s="5"/>
     </row>
@@ -3818,11 +3864,11 @@
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>0.51020408163265307</v>
+        <v>0.46296296296296291</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
@@ -3917,40 +3963,42 @@
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>0.92857142857142849</v>
+        <v>0.84259259259259256</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="AH34" s="1"/>
+      <c r="AH34" s="1">
+        <v>1</v>
+      </c>
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL34" s="1">
         <v>3</v>
       </c>
       <c r="AM34" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN34" s="4">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO34" s="8">
         <v>0</v>
       </c>
       <c r="AP34" s="4">
         <f t="shared" si="9"/>
-        <v>1.6666666666666667</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ34" s="5"/>
     </row>
@@ -3982,7 +4030,9 @@
         <v>1</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -3992,7 +4042,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1">
         <f t="shared" ref="T35" si="10">SUM(C35:S35)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U35" s="1">
         <v>0.2</v>
@@ -4016,11 +4066,11 @@
       </c>
       <c r="AD35" s="1">
         <f t="shared" ref="AD35" si="12">T35+AC35</f>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AE35" s="4">
         <f>AD35</f>
-        <v>9.8000000000000007</v>
+        <v>10.8</v>
       </c>
       <c r="AF35" s="7">
         <f t="shared" ref="AF35" si="13">(AD35/AE35)</f>
@@ -4030,30 +4080,32 @@
         <f t="shared" ref="AG35" si="14">MAX(IF(AF35*100&gt;=20,2,0),IF(AF35*100&gt;=40,3,0),IF(AF35*100&gt;=60,4,0),IF(AF35*100&gt;=80,5,0))</f>
         <v>5</v>
       </c>
-      <c r="AH35" s="1"/>
+      <c r="AH35" s="1">
+        <v>1</v>
+      </c>
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1">
         <f t="shared" ref="AK35" si="15">SUM(AH35:AJ35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL35" s="9">
         <v>3</v>
       </c>
       <c r="AM35" s="4">
         <f t="shared" ref="AM35" si="16">(AK35/AL35)*100</f>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN35" s="4">
         <f t="shared" ref="AN35" si="17">MAX(IF(AM35&gt;=20,2,0),IF(AM35&gt;=40,3,0),IF(AM35&gt;=60,4,0),IF(AM35&gt;=80,5,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO35" s="8">
         <v>0</v>
       </c>
       <c r="AP35" s="4">
         <f t="shared" ref="AP35" si="18">(AG35+AN35+AO35)/3</f>
-        <v>1.6666666666666667</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ35" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update achievement. Update exam questions.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5D1D5-CF7D-42B9-BE3D-3C713BEBDEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2553995A-95F8-4CC7-8689-60303FA2CF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -604,7 +604,7 @@
     <col min="6" max="6" width="3.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="13" max="19" width="4.296875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.8984375" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="4.296875" bestFit="1" customWidth="1"/>
@@ -783,7 +783,9 @@
         <v>0.6</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="L2" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -793,7 +795,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f t="shared" ref="T2:T34" si="0">SUM(C2:S2)</f>
-        <v>5.4499999999999993</v>
+        <v>5.7499999999999991</v>
       </c>
       <c r="U2" s="9">
         <v>0.1</v>
@@ -803,25 +805,27 @@
       <c r="X2" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y2" s="1"/>
+      <c r="Y2" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1">
         <f t="shared" ref="AC2:AC34" si="1">SUM(U2:AB2)</f>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD2" s="1">
         <f t="shared" ref="AD2:AD34" si="2">T2+AC2</f>
-        <v>5.6499999999999995</v>
+        <v>6.0499999999999989</v>
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.52314814814814803</v>
+        <v>0.50416666666666654</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
@@ -914,11 +918,11 @@
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>0.44444444444444442</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
@@ -1009,15 +1013,15 @@
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.40277777777777773</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH4" s="1">
         <v>0.5</v>
@@ -1044,7 +1048,7 @@
       </c>
       <c r="AP4" s="4">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="AQ4" s="5"/>
     </row>
@@ -1072,7 +1076,9 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="L5" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1082,7 +1088,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1">
         <f t="shared" si="0"/>
-        <v>4.6999999999999993</v>
+        <v>4.9999999999999991</v>
       </c>
       <c r="U5" s="9">
         <v>0.1</v>
@@ -1100,15 +1106,15 @@
       </c>
       <c r="AD5" s="1">
         <f t="shared" si="2"/>
-        <v>4.7999999999999989</v>
+        <v>5.0999999999999988</v>
       </c>
       <c r="AE5" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="4"/>
-        <v>0.44444444444444431</v>
+        <v>0.42499999999999988</v>
       </c>
       <c r="AG5" s="4">
         <f t="shared" si="5"/>
@@ -1165,7 +1171,9 @@
         <v>0.1</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="1">
+        <v>0.2</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1175,7 +1183,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>3.95</v>
       </c>
       <c r="U6" s="9">
         <v>0</v>
@@ -1183,25 +1191,27 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
+      <c r="Y6" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD6" s="1">
         <f t="shared" si="2"/>
-        <v>3.75</v>
+        <v>4.05</v>
       </c>
       <c r="AE6" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF6" s="7">
         <f t="shared" si="4"/>
-        <v>0.34722222222222221</v>
+        <v>0.33749999999999997</v>
       </c>
       <c r="AG6" s="4">
         <f t="shared" si="5"/>
@@ -1264,7 +1274,9 @@
         <v>0.6</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1274,7 +1286,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>7.6999999999999993</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="U7" s="9">
         <v>0</v>
@@ -1284,25 +1296,27 @@
       <c r="X7" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y7" s="1"/>
+      <c r="Y7" s="1">
+        <v>0.2</v>
+      </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="2"/>
-        <v>7.7999999999999989</v>
+        <v>9</v>
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>0.7222222222222221</v>
+        <v>0.75</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
@@ -1363,7 +1377,9 @@
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1373,7 +1389,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1">
         <f t="shared" si="0"/>
-        <v>5.85</v>
+        <v>6.1499999999999995</v>
       </c>
       <c r="U8" s="9">
         <v>0</v>
@@ -1383,25 +1399,27 @@
       <c r="X8" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y8" s="1"/>
+      <c r="Y8" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD8" s="1">
         <f t="shared" si="2"/>
-        <v>5.9499999999999993</v>
+        <v>6.4499999999999993</v>
       </c>
       <c r="AE8" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF8" s="7">
         <f t="shared" si="4"/>
-        <v>0.55092592592592582</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" si="5"/>
@@ -1458,7 +1476,9 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1468,7 +1488,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1">
         <f t="shared" si="0"/>
-        <v>4.6500000000000004</v>
+        <v>4.95</v>
       </c>
       <c r="U9" s="1">
         <v>0.2</v>
@@ -1488,15 +1508,15 @@
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="2"/>
-        <v>4.95</v>
+        <v>5.25</v>
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>0.45833333333333331</v>
+        <v>0.4375</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
@@ -1557,7 +1577,9 @@
         <v>0.6</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1567,7 +1589,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1">
         <f t="shared" si="0"/>
-        <v>8.1</v>
+        <v>9.1</v>
       </c>
       <c r="U10" s="9">
         <v>0.1</v>
@@ -1577,25 +1599,27 @@
       <c r="X10" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y10" s="1"/>
+      <c r="Y10" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD10" s="1">
         <f t="shared" si="2"/>
-        <v>8.2999999999999989</v>
+        <v>9.4</v>
       </c>
       <c r="AE10" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF10" s="7">
         <f t="shared" si="4"/>
-        <v>0.76851851851851838</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="AG10" s="4">
         <f t="shared" si="5"/>
@@ -1656,7 +1680,9 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1666,7 +1692,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1">
         <f t="shared" si="0"/>
-        <v>6.55</v>
+        <v>7.55</v>
       </c>
       <c r="U11" s="9">
         <v>0</v>
@@ -1684,15 +1710,15 @@
       </c>
       <c r="AD11" s="1">
         <f t="shared" si="2"/>
-        <v>6.55</v>
+        <v>7.55</v>
       </c>
       <c r="AE11" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF11" s="7">
         <f t="shared" si="4"/>
-        <v>0.6064814814814814</v>
+        <v>0.62916666666666665</v>
       </c>
       <c r="AG11" s="4">
         <f t="shared" si="5"/>
@@ -1789,15 +1815,15 @@
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>0.60185185185185186</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH12" s="1">
         <v>0.5</v>
@@ -1824,7 +1850,7 @@
       </c>
       <c r="AP12" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ12" s="5"/>
     </row>
@@ -1859,7 +1885,9 @@
       <c r="L13" s="1">
         <v>0.6</v>
       </c>
-      <c r="M13" s="1"/>
+      <c r="M13" s="1">
+        <v>0.3</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1868,7 +1896,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1">
         <f t="shared" si="0"/>
-        <v>5.7999999999999989</v>
+        <v>6.0999999999999988</v>
       </c>
       <c r="U13" s="9">
         <v>0</v>
@@ -1888,15 +1916,15 @@
       </c>
       <c r="AD13" s="1">
         <f t="shared" si="2"/>
-        <v>5.8999999999999986</v>
+        <v>6.1999999999999984</v>
       </c>
       <c r="AE13" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF13" s="7">
         <f t="shared" si="4"/>
-        <v>0.54629629629629617</v>
+        <v>0.5166666666666665</v>
       </c>
       <c r="AG13" s="4">
         <f t="shared" si="5"/>
@@ -1957,7 +1985,9 @@
         <v>1</v>
       </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1967,7 +1997,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U14" s="9">
         <v>0.2</v>
@@ -1979,25 +2009,27 @@
       <c r="X14" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y14" s="1"/>
+      <c r="Y14" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="AD14" s="1">
         <f t="shared" si="2"/>
-        <v>7.4</v>
+        <v>8.6</v>
       </c>
       <c r="AE14" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF14" s="7">
         <f t="shared" si="4"/>
-        <v>0.68518518518518512</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="AG14" s="4">
         <f t="shared" si="5"/>
@@ -2058,7 +2090,9 @@
         <v>0.3</v>
       </c>
       <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="1">
+        <v>0.6</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -2068,7 +2102,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1">
         <f t="shared" si="0"/>
-        <v>4.8500000000000005</v>
+        <v>5.45</v>
       </c>
       <c r="U15" s="9">
         <v>0</v>
@@ -2086,15 +2120,15 @@
       </c>
       <c r="AD15" s="1">
         <f t="shared" si="2"/>
-        <v>4.8500000000000005</v>
+        <v>5.45</v>
       </c>
       <c r="AE15" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF15" s="7">
         <f t="shared" si="4"/>
-        <v>0.44907407407407407</v>
+        <v>0.45416666666666666</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="5"/>
@@ -2191,15 +2225,15 @@
       </c>
       <c r="AE16" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF16" s="7">
         <f t="shared" si="4"/>
-        <v>0.66203703703703698</v>
+        <v>0.59583333333333333</v>
       </c>
       <c r="AG16" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AH16" s="1">
         <v>0.5</v>
@@ -2226,7 +2260,7 @@
       </c>
       <c r="AP16" s="4">
         <f t="shared" si="9"/>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AQ16" s="5"/>
     </row>
@@ -2254,7 +2288,9 @@
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="L17" s="1">
+        <v>0.6</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -2264,7 +2300,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>5.35</v>
       </c>
       <c r="U17" s="9">
         <v>0.1</v>
@@ -2274,25 +2310,27 @@
       <c r="X17" s="1">
         <v>0.1</v>
       </c>
-      <c r="Y17" s="1"/>
+      <c r="Y17" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AD17" s="1">
         <f t="shared" si="2"/>
-        <v>4.95</v>
+        <v>5.6499999999999995</v>
       </c>
       <c r="AE17" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF17" s="7">
         <f t="shared" si="4"/>
-        <v>0.45833333333333331</v>
+        <v>0.47083333333333327</v>
       </c>
       <c r="AG17" s="4">
         <f t="shared" si="5"/>
@@ -2349,7 +2387,9 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -2359,7 +2399,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1">
         <f t="shared" si="0"/>
-        <v>4.6500000000000004</v>
+        <v>4.95</v>
       </c>
       <c r="U18" s="9">
         <v>0</v>
@@ -2377,15 +2417,15 @@
       </c>
       <c r="AD18" s="1">
         <f t="shared" si="2"/>
-        <v>4.6500000000000004</v>
+        <v>4.95</v>
       </c>
       <c r="AE18" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF18" s="7">
         <f t="shared" si="4"/>
-        <v>0.43055555555555558</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" si="5"/>
@@ -2446,7 +2486,9 @@
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="L19" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -2456,7 +2498,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1">
         <f t="shared" si="0"/>
-        <v>6.6</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="U19" s="9">
         <v>0.1</v>
@@ -2468,25 +2510,27 @@
       <c r="X19" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y19" s="1"/>
+      <c r="Y19" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="2"/>
-        <v>6.8999999999999995</v>
+        <v>7.3999999999999995</v>
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>0.63888888888888884</v>
+        <v>0.61666666666666659</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
@@ -2591,11 +2635,11 @@
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>1.0555555555555556</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
@@ -2654,7 +2698,9 @@
         <v>0.1</v>
       </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="L21" s="1">
+        <v>0.1</v>
+      </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -2664,7 +2710,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1">
         <f t="shared" si="0"/>
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
       <c r="U21" s="9">
         <v>0</v>
@@ -2682,15 +2728,15 @@
       </c>
       <c r="AD21" s="1">
         <f t="shared" si="2"/>
-        <v>3.75</v>
+        <v>3.85</v>
       </c>
       <c r="AE21" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF21" s="7">
         <f t="shared" si="4"/>
-        <v>0.34722222222222221</v>
+        <v>0.32083333333333336</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="5"/>
@@ -2751,7 +2797,9 @@
         <v>0.6</v>
       </c>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="L22" s="1">
+        <v>0.3</v>
+      </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -2761,7 +2809,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1">
         <f t="shared" si="0"/>
-        <v>8.1</v>
+        <v>8.4</v>
       </c>
       <c r="U22" s="1">
         <v>0.1</v>
@@ -2773,25 +2821,27 @@
       <c r="X22" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y22" s="1"/>
+      <c r="Y22" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="2"/>
-        <v>8.4</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>0.77777777777777779</v>
+        <v>0.73333333333333339</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
@@ -2878,11 +2928,11 @@
       </c>
       <c r="AE23" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF23" s="7">
         <f t="shared" si="4"/>
-        <v>0.32407407407407407</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="AG23" s="8">
         <f t="shared" si="5"/>
@@ -2943,7 +2993,9 @@
         <v>1</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -2953,7 +3005,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1">
         <f t="shared" si="0"/>
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="U24" s="9">
         <v>0</v>
@@ -2963,29 +3015,31 @@
       <c r="X24" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="1">
+        <v>0.1</v>
+      </c>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
       <c r="AC24" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD24" s="1">
         <f t="shared" si="2"/>
-        <v>8.6</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>0.79629629629629617</v>
+        <v>0.80833333333333324</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH24" s="1">
         <v>1</v>
@@ -3012,7 +3066,7 @@
       </c>
       <c r="AP24" s="4">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ24" s="5"/>
     </row>
@@ -3072,11 +3126,11 @@
       </c>
       <c r="AE25" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF25" s="7">
         <f t="shared" si="4"/>
-        <v>0.4861111111111111</v>
+        <v>0.4375</v>
       </c>
       <c r="AG25" s="4">
         <f t="shared" si="5"/>
@@ -3137,7 +3191,9 @@
         <v>1</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -3147,7 +3203,7 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U26" s="9">
         <v>0</v>
@@ -3169,15 +3225,15 @@
       </c>
       <c r="AD26" s="1">
         <f t="shared" si="2"/>
-        <v>9.1999999999999993</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AE26" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF26" s="7">
         <f t="shared" si="4"/>
-        <v>0.85185185185185175</v>
+        <v>0.85</v>
       </c>
       <c r="AG26" s="4">
         <f t="shared" si="5"/>
@@ -3246,7 +3302,9 @@
       <c r="M27" s="1">
         <v>1</v>
       </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="1">
+        <v>1.5</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -3254,7 +3312,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="U27" s="9">
         <v>0.2</v>
@@ -3268,25 +3326,27 @@
       <c r="X27" s="9">
         <v>0.2</v>
       </c>
-      <c r="Y27" s="1"/>
+      <c r="Y27" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
       <c r="AC27" s="1">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="2"/>
-        <v>11.7</v>
+        <v>13.4</v>
       </c>
       <c r="AE27" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF27" s="7">
         <f t="shared" si="4"/>
-        <v>1.0833333333333333</v>
+        <v>1.1166666666666667</v>
       </c>
       <c r="AG27" s="4">
         <f t="shared" si="5"/>
@@ -3343,7 +3403,9 @@
         <v>0.6</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="1">
+        <v>0.45</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -3353,7 +3415,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1">
         <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="U28" s="9">
         <v>0.2</v>
@@ -3365,25 +3427,27 @@
       <c r="X28" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y28" s="1"/>
+      <c r="Y28" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
       <c r="AC28" s="1">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AD28" s="1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>5.55</v>
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>0.46296296296296291</v>
+        <v>0.46249999999999997</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
@@ -3446,7 +3510,9 @@
         <v>0.3</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="L29" s="1">
+        <v>0.35</v>
+      </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -3456,7 +3522,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1">
         <f t="shared" si="0"/>
-        <v>6.1999999999999993</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="U29" s="9">
         <v>0</v>
@@ -3476,15 +3542,15 @@
       </c>
       <c r="AD29" s="1">
         <f t="shared" si="2"/>
-        <v>6.2999999999999989</v>
+        <v>6.6499999999999986</v>
       </c>
       <c r="AE29" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF29" s="7">
         <f t="shared" si="4"/>
-        <v>0.58333333333333315</v>
+        <v>0.55416666666666659</v>
       </c>
       <c r="AG29" s="4">
         <f t="shared" si="5"/>
@@ -3520,24 +3586,22 @@
     <row r="30" spans="1:43" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F30" s="1">
         <v>1.5</v>
       </c>
       <c r="G30" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0.6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -3551,7 +3615,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="U30" s="9">
         <v>0</v>
@@ -3569,15 +3633,15 @@
       </c>
       <c r="AD30" s="1">
         <f t="shared" si="2"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="AE30" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF30" s="7">
         <f t="shared" si="4"/>
-        <v>0.43981481481481477</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="AG30" s="4">
         <f t="shared" si="5"/>
@@ -3613,32 +3677,30 @@
     <row r="31" spans="1:43" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F31" s="9">
         <v>1.5</v>
       </c>
       <c r="G31" s="1">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="H31" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1</v>
-      </c>
-      <c r="J31" s="1">
         <v>0.6</v>
       </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="L31" s="1">
+        <v>0.2</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -3648,75 +3710,69 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1">
         <f t="shared" si="0"/>
-        <v>8.1</v>
+        <v>4.95</v>
       </c>
       <c r="U31" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="V31" s="1">
-        <v>0.1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="V31" s="1"/>
       <c r="W31" s="1"/>
-      <c r="X31" s="9">
-        <v>0.2</v>
-      </c>
+      <c r="X31" s="9"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
       <c r="AC31" s="1">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AD31" s="1">
         <f t="shared" si="2"/>
-        <v>8.6</v>
+        <v>4.95</v>
       </c>
       <c r="AE31" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF31" s="7">
         <f t="shared" si="4"/>
-        <v>0.79629629629629617</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="AG31" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AH31" s="1">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL31" s="1">
         <v>3</v>
       </c>
       <c r="AM31" s="4">
         <f t="shared" si="7"/>
-        <v>33.333333333333329</v>
+        <v>0</v>
       </c>
       <c r="AN31" s="4">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="8">
         <v>0</v>
       </c>
       <c r="AP31" s="4">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ31" s="5"/>
     </row>
     <row r="32" spans="1:43" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9">
@@ -3729,19 +3785,21 @@
         <v>1.5</v>
       </c>
       <c r="G32" s="9">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="H32" s="9">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I32" s="9">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="J32" s="9">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
+      <c r="L32" s="9">
+        <v>1</v>
+      </c>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
       <c r="O32" s="9"/>
@@ -3751,69 +3809,77 @@
       <c r="S32" s="9"/>
       <c r="T32" s="9">
         <f t="shared" si="0"/>
-        <v>6.05</v>
+        <v>9.1</v>
       </c>
       <c r="U32" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="V32" s="9">
         <v>0.1</v>
       </c>
-      <c r="V32" s="9"/>
       <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
+      <c r="X32" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="Y32" s="9">
+        <v>0.2</v>
+      </c>
       <c r="Z32" s="9"/>
       <c r="AA32" s="9"/>
       <c r="AB32" s="9"/>
       <c r="AC32" s="9">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="AD32" s="9">
         <f t="shared" si="2"/>
-        <v>6.1499999999999995</v>
+        <v>9.7999999999999989</v>
       </c>
       <c r="AE32" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF32" s="7">
         <f t="shared" si="4"/>
-        <v>0.56944444444444431</v>
+        <v>0.81666666666666654</v>
       </c>
       <c r="AG32" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="AH32" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="AH32" s="9">
+        <v>1</v>
+      </c>
       <c r="AI32" s="9"/>
       <c r="AJ32" s="9"/>
       <c r="AK32" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL32" s="9">
         <v>3</v>
       </c>
       <c r="AM32" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="AN32" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AO32" s="8">
         <v>0</v>
       </c>
       <c r="AP32" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="AQ32" s="5"/>
     </row>
     <row r="33" spans="1:43" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9">
@@ -3826,13 +3892,21 @@
         <v>1.5</v>
       </c>
       <c r="G33" s="9">
-        <v>1</v>
-      </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+        <v>0.65</v>
+      </c>
+      <c r="H33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.1</v>
+      </c>
       <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
+      <c r="L33" s="9">
+        <v>1</v>
+      </c>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
@@ -3842,10 +3916,10 @@
       <c r="S33" s="9"/>
       <c r="T33" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7.05</v>
       </c>
       <c r="U33" s="9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="V33" s="9"/>
       <c r="W33" s="9"/>
@@ -3856,19 +3930,19 @@
       <c r="AB33" s="9"/>
       <c r="AC33" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AD33" s="9">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>0.46296296296296291</v>
+        <v>0.59583333333333333</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
@@ -3929,7 +4003,9 @@
         <v>1</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="L34" s="1">
+        <v>1</v>
+      </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -3939,7 +4015,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="U34" s="9">
         <v>0</v>
@@ -3949,25 +4025,27 @@
       <c r="X34" s="9">
         <v>0.1</v>
       </c>
-      <c r="Y34" s="1"/>
+      <c r="Y34" s="9">
+        <v>0.1</v>
+      </c>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
       <c r="AC34" s="1">
         <f t="shared" si="1"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="AD34" s="1">
         <f t="shared" si="2"/>
-        <v>9.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>0.84259259259259256</v>
+        <v>0.85</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>
@@ -4033,7 +4111,9 @@
       <c r="L35" s="1">
         <v>1</v>
       </c>
-      <c r="M35" s="1"/>
+      <c r="M35" s="1">
+        <v>1</v>
+      </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -4042,7 +4122,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1">
         <f t="shared" ref="T35" si="10">SUM(C35:S35)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U35" s="1">
         <v>0.2</v>
@@ -4056,21 +4136,23 @@
       <c r="X35" s="1">
         <v>0.2</v>
       </c>
-      <c r="Y35" s="1"/>
+      <c r="Y35" s="1">
+        <v>0.2</v>
+      </c>
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
       <c r="AC35" s="1">
         <f t="shared" ref="AC35" si="11">SUM(U35:AB35)</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AD35" s="1">
         <f t="shared" ref="AD35" si="12">T35+AC35</f>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AE35" s="4">
         <f>AD35</f>
-        <v>10.8</v>
+        <v>12</v>
       </c>
       <c r="AF35" s="7">
         <f t="shared" ref="AF35" si="13">(AD35/AE35)</f>

</xml_diff>

<commit_message>
Update achievement. Add tasks.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9602CD1F-62AB-4232-85E2-004816451FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED0BAD7-54B6-40D3-ACC1-7169E0DE8EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="МК-101" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -590,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -786,7 +787,9 @@
       <c r="L2" s="1">
         <v>0.3</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1">
+        <v>0.1</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -795,7 +798,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1">
         <f t="shared" ref="T2:T34" si="0">SUM(C2:S2)</f>
-        <v>5.7499999999999991</v>
+        <v>5.8499999999999988</v>
       </c>
       <c r="U2" s="9">
         <v>0.1</v>
@@ -817,7 +820,7 @@
       </c>
       <c r="AD2" s="1">
         <f t="shared" ref="AD2:AD34" si="2">T2+AC2</f>
-        <v>6.0499999999999989</v>
+        <v>6.1499999999999986</v>
       </c>
       <c r="AE2" s="9">
         <f t="shared" ref="AE2:AE34" si="3">AE3</f>
@@ -825,7 +828,7 @@
       </c>
       <c r="AF2" s="7">
         <f t="shared" ref="AF2:AF34" si="4">(AD2/AE2)</f>
-        <v>0.49590163934426224</v>
+        <v>0.50409836065573765</v>
       </c>
       <c r="AG2" s="4">
         <f t="shared" ref="AG2:AG34" si="5">MAX(IF(AF2*100&gt;=20,2,0),IF(AF2*100&gt;=40,3,0),IF(AF2*100&gt;=60,4,0),IF(AF2*100&gt;=80,5,0))</f>
@@ -885,7 +888,9 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="M3" s="1">
+        <v>0.1</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -894,7 +899,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="U3" s="1">
         <v>0</v>
@@ -914,7 +919,7 @@
       </c>
       <c r="AD3" s="1">
         <f t="shared" si="2"/>
-        <v>4.8</v>
+        <v>4.8999999999999995</v>
       </c>
       <c r="AE3" s="9">
         <f t="shared" si="3"/>
@@ -922,11 +927,11 @@
       </c>
       <c r="AF3" s="7">
         <f t="shared" si="4"/>
-        <v>0.39344262295081966</v>
+        <v>0.40163934426229508</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -951,7 +956,7 @@
       </c>
       <c r="AP3" s="4">
         <f t="shared" si="9"/>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="AQ3" s="5"/>
     </row>
@@ -980,7 +985,9 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1">
+        <v>0.1</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -989,7 +996,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="U4" s="9">
         <v>0</v>
@@ -1009,7 +1016,7 @@
       </c>
       <c r="AD4" s="1">
         <f t="shared" si="2"/>
-        <v>4.3499999999999996</v>
+        <v>4.4499999999999993</v>
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="3"/>
@@ -1017,7 +1024,7 @@
       </c>
       <c r="AF4" s="7">
         <f t="shared" si="4"/>
-        <v>0.35655737704918034</v>
+        <v>0.3647540983606557</v>
       </c>
       <c r="AG4" s="4">
         <f t="shared" si="5"/>
@@ -1279,7 +1286,9 @@
       <c r="L7" s="1">
         <v>1</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1">
+        <v>0.6</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1288,7 +1297,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1">
         <f t="shared" si="0"/>
-        <v>8.6999999999999993</v>
+        <v>9.2999999999999989</v>
       </c>
       <c r="U7" s="9">
         <v>0</v>
@@ -1310,7 +1319,7 @@
       </c>
       <c r="AD7" s="1">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>9.6</v>
       </c>
       <c r="AE7" s="9">
         <f t="shared" si="3"/>
@@ -1318,7 +1327,7 @@
       </c>
       <c r="AF7" s="7">
         <f t="shared" si="4"/>
-        <v>0.73770491803278693</v>
+        <v>0.78688524590163933</v>
       </c>
       <c r="AG7" s="4">
         <f t="shared" si="5"/>
@@ -1481,7 +1490,9 @@
       <c r="L9" s="1">
         <v>0.3</v>
       </c>
-      <c r="M9" s="1"/>
+      <c r="M9" s="1">
+        <v>0.1</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1490,7 +1501,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1">
         <f t="shared" si="0"/>
-        <v>4.95</v>
+        <v>5.05</v>
       </c>
       <c r="U9" s="1">
         <v>0.2</v>
@@ -1510,7 +1521,7 @@
       </c>
       <c r="AD9" s="1">
         <f t="shared" si="2"/>
-        <v>5.25</v>
+        <v>5.35</v>
       </c>
       <c r="AE9" s="9">
         <f t="shared" si="3"/>
@@ -1518,7 +1529,7 @@
       </c>
       <c r="AF9" s="7">
         <f t="shared" si="4"/>
-        <v>0.43032786885245905</v>
+        <v>0.43852459016393441</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="5"/>
@@ -1782,7 +1793,9 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="M12" s="1">
+        <v>0.1</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1791,7 +1804,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1">
         <f t="shared" si="0"/>
-        <v>6.3</v>
+        <v>6.3999999999999995</v>
       </c>
       <c r="U12" s="9">
         <v>0</v>
@@ -1813,7 +1826,7 @@
       </c>
       <c r="AD12" s="1">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="AE12" s="9">
         <f t="shared" si="3"/>
@@ -1821,7 +1834,7 @@
       </c>
       <c r="AF12" s="7">
         <f t="shared" si="4"/>
-        <v>0.53278688524590168</v>
+        <v>0.54098360655737709</v>
       </c>
       <c r="AG12" s="4">
         <f t="shared" si="5"/>
@@ -2497,7 +2510,9 @@
       <c r="L19" s="1">
         <v>0.3</v>
       </c>
-      <c r="M19" s="1"/>
+      <c r="M19" s="1">
+        <v>0.1</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -2506,7 +2521,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1">
         <f t="shared" si="0"/>
-        <v>6.8999999999999995</v>
+        <v>6.9999999999999991</v>
       </c>
       <c r="U19" s="9">
         <v>0.1</v>
@@ -2530,7 +2545,7 @@
       </c>
       <c r="AD19" s="1">
         <f t="shared" si="2"/>
-        <v>7.3999999999999995</v>
+        <v>7.4999999999999991</v>
       </c>
       <c r="AE19" s="9">
         <f t="shared" si="3"/>
@@ -2538,7 +2553,7 @@
       </c>
       <c r="AF19" s="7">
         <f t="shared" si="4"/>
-        <v>0.60655737704918034</v>
+        <v>0.61475409836065575</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="5"/>
@@ -2607,7 +2622,9 @@
       <c r="M20" s="1">
         <v>1</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>1.5</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -2615,7 +2632,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="U20" s="9">
         <v>0.1</v>
@@ -2641,7 +2658,7 @@
       </c>
       <c r="AD20" s="1">
         <f t="shared" si="2"/>
-        <v>11.5</v>
+        <v>13</v>
       </c>
       <c r="AE20" s="9">
         <f t="shared" si="3"/>
@@ -2649,7 +2666,7 @@
       </c>
       <c r="AF20" s="7">
         <f t="shared" si="4"/>
-        <v>0.94262295081967218</v>
+        <v>1.0655737704918034</v>
       </c>
       <c r="AG20" s="4">
         <f t="shared" si="5"/>
@@ -2810,7 +2827,9 @@
       <c r="L22" s="1">
         <v>0.3</v>
       </c>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1">
+        <v>0.3</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -2819,7 +2838,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1">
         <f t="shared" si="0"/>
-        <v>8.4</v>
+        <v>8.7000000000000011</v>
       </c>
       <c r="U22" s="1">
         <v>0.1</v>
@@ -2843,7 +2862,7 @@
       </c>
       <c r="AD22" s="1">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
+        <v>9.1000000000000014</v>
       </c>
       <c r="AE22" s="9">
         <f t="shared" si="3"/>
@@ -2851,7 +2870,7 @@
       </c>
       <c r="AF22" s="7">
         <f t="shared" si="4"/>
-        <v>0.7213114754098362</v>
+        <v>0.74590163934426246</v>
       </c>
       <c r="AG22" s="4">
         <f t="shared" si="5"/>
@@ -3006,7 +3025,9 @@
       <c r="L24" s="1">
         <v>1</v>
       </c>
-      <c r="M24" s="1"/>
+      <c r="M24" s="1">
+        <v>0.6</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -3015,7 +3036,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1">
         <f t="shared" si="0"/>
-        <v>9.5</v>
+        <v>10.1</v>
       </c>
       <c r="U24" s="9">
         <v>0</v>
@@ -3039,7 +3060,7 @@
       </c>
       <c r="AD24" s="1">
         <f t="shared" si="2"/>
-        <v>9.8000000000000007</v>
+        <v>10.4</v>
       </c>
       <c r="AE24" s="9">
         <f t="shared" si="3"/>
@@ -3047,7 +3068,7 @@
       </c>
       <c r="AF24" s="7">
         <f t="shared" si="4"/>
-        <v>0.80327868852459028</v>
+        <v>0.85245901639344268</v>
       </c>
       <c r="AG24" s="4">
         <f t="shared" si="5"/>
@@ -3420,7 +3441,9 @@
       <c r="L28" s="1">
         <v>0.45</v>
       </c>
-      <c r="M28" s="1"/>
+      <c r="M28" s="1">
+        <v>0.3</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3429,7 +3452,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1">
         <f t="shared" si="0"/>
-        <v>5.05</v>
+        <v>5.35</v>
       </c>
       <c r="U28" s="9">
         <v>0.2</v>
@@ -3455,7 +3478,7 @@
       </c>
       <c r="AD28" s="1">
         <f t="shared" si="2"/>
-        <v>5.6499999999999995</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="AE28" s="9">
         <f t="shared" si="3"/>
@@ -3463,7 +3486,7 @@
       </c>
       <c r="AF28" s="7">
         <f t="shared" si="4"/>
-        <v>0.46311475409836061</v>
+        <v>0.48770491803278687</v>
       </c>
       <c r="AG28" s="4">
         <f t="shared" si="5"/>
@@ -3923,7 +3946,9 @@
       <c r="L33" s="9">
         <v>1</v>
       </c>
-      <c r="M33" s="9"/>
+      <c r="M33" s="9">
+        <v>0.6</v>
+      </c>
       <c r="N33" s="9"/>
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
@@ -3932,7 +3957,7 @@
       <c r="S33" s="9"/>
       <c r="T33" s="9">
         <f t="shared" si="0"/>
-        <v>7.05</v>
+        <v>7.6499999999999995</v>
       </c>
       <c r="U33" s="9">
         <v>0.1</v>
@@ -3950,7 +3975,7 @@
       </c>
       <c r="AD33" s="9">
         <f t="shared" si="2"/>
-        <v>7.1499999999999995</v>
+        <v>7.7499999999999991</v>
       </c>
       <c r="AE33" s="9">
         <f t="shared" si="3"/>
@@ -3958,11 +3983,11 @@
       </c>
       <c r="AF33" s="7">
         <f t="shared" si="4"/>
-        <v>0.58606557377049184</v>
+        <v>0.63524590163934425</v>
       </c>
       <c r="AG33" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH33" s="9"/>
       <c r="AI33" s="9"/>
@@ -3987,7 +4012,7 @@
       </c>
       <c r="AP33" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="AQ33" s="5"/>
     </row>
@@ -4022,7 +4047,9 @@
       <c r="L34" s="1">
         <v>1</v>
       </c>
-      <c r="M34" s="1"/>
+      <c r="M34" s="1">
+        <v>0.6</v>
+      </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
@@ -4031,7 +4058,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>10.6</v>
       </c>
       <c r="U34" s="9">
         <v>0</v>
@@ -4055,7 +4082,7 @@
       </c>
       <c r="AD34" s="1">
         <f t="shared" si="2"/>
-        <v>10.3</v>
+        <v>10.9</v>
       </c>
       <c r="AE34" s="1">
         <f t="shared" si="3"/>
@@ -4063,7 +4090,7 @@
       </c>
       <c r="AF34" s="7">
         <f t="shared" si="4"/>
-        <v>0.84426229508196737</v>
+        <v>0.89344262295081978</v>
       </c>
       <c r="AG34" s="4">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
Update achievement. Add task.
</commit_message>
<xml_diff>
--- a/Успеваемость.xlsx
+++ b/Успеваемость.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAIN\repositories\github\csu\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347C1D7-48FE-4DD4-98C2-F678FBC4C6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AB52B8-8E9B-44B6-9A5C-208B9E1EA069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -874,11 +874,11 @@
       </c>
       <c r="AK2" s="1">
         <f t="shared" ref="AK2:AK34" si="2">AK3</f>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL2" s="7">
         <f t="shared" ref="AL2:AL34" si="3">(AJ2/AK2)</f>
-        <v>0.37239583333333331</v>
+        <v>0.36855670103092786</v>
       </c>
       <c r="AM2" s="4">
         <f t="shared" ref="AM2:AM34" si="4">MAX(IF(AL2*100&gt;=20,2,0),IF(AL2*100&gt;=40,3,0),IF(AL2*100&gt;=60,4,0),IF(AL2*100&gt;=80,5,0))</f>
@@ -949,13 +949,15 @@
       <c r="Q3" s="1">
         <v>0.2</v>
       </c>
-      <c r="R3" s="1"/>
+      <c r="R3" s="1">
+        <v>0.3</v>
+      </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1">
         <f t="shared" si="0"/>
-        <v>5.05</v>
+        <v>5.35</v>
       </c>
       <c r="W3" s="1">
         <v>0</v>
@@ -979,15 +981,15 @@
       </c>
       <c r="AJ3" s="1">
         <f t="shared" si="1"/>
-        <v>5.0999999999999996</v>
+        <v>5.3999999999999995</v>
       </c>
       <c r="AK3" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL3" s="7">
         <f t="shared" si="3"/>
-        <v>0.265625</v>
+        <v>0.27835051546391754</v>
       </c>
       <c r="AM3" s="4">
         <f t="shared" si="4"/>
@@ -1085,22 +1087,24 @@
       <c r="AG4" s="1">
         <v>0.1</v>
       </c>
-      <c r="AH4" s="1"/>
+      <c r="AH4" s="1">
+        <v>0.1</v>
+      </c>
       <c r="AI4" s="1">
         <f t="shared" si="9"/>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="1"/>
-        <v>5.45</v>
+        <v>5.5500000000000007</v>
       </c>
       <c r="AK4" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL4" s="7">
         <f t="shared" si="3"/>
-        <v>0.28385416666666669</v>
+        <v>0.28608247422680416</v>
       </c>
       <c r="AM4" s="4">
         <f t="shared" si="4"/>
@@ -1205,11 +1209,11 @@
       </c>
       <c r="AK5" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL5" s="7">
         <f t="shared" si="3"/>
-        <v>0.27604166666666663</v>
+        <v>0.27319587628865977</v>
       </c>
       <c r="AM5" s="4">
         <f t="shared" si="4"/>
@@ -1308,11 +1312,11 @@
       </c>
       <c r="AK6" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL6" s="7">
         <f t="shared" si="3"/>
-        <v>0.2109375</v>
+        <v>0.20876288659793815</v>
       </c>
       <c r="AM6" s="4">
         <f t="shared" si="4"/>
@@ -1391,13 +1395,15 @@
       <c r="Q7" s="1">
         <v>1</v>
       </c>
-      <c r="R7" s="1"/>
+      <c r="R7" s="1">
+        <v>1.3</v>
+      </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1">
         <f t="shared" si="0"/>
-        <v>11.749999999999998</v>
+        <v>13.049999999999999</v>
       </c>
       <c r="W7" s="1">
         <v>0</v>
@@ -1427,15 +1433,15 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="1"/>
-        <v>12.249999999999998</v>
+        <v>13.549999999999999</v>
       </c>
       <c r="AK7" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL7" s="7">
         <f t="shared" si="3"/>
-        <v>0.63802083333333326</v>
+        <v>0.69845360824742264</v>
       </c>
       <c r="AM7" s="4">
         <f t="shared" si="4"/>
@@ -1542,11 +1548,11 @@
       </c>
       <c r="AK8" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL8" s="7">
         <f t="shared" si="3"/>
-        <v>0.35416666666666669</v>
+        <v>0.3505154639175258</v>
       </c>
       <c r="AM8" s="4">
         <f t="shared" si="4"/>
@@ -1649,11 +1655,11 @@
       </c>
       <c r="AK9" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL9" s="7">
         <f t="shared" si="3"/>
-        <v>0.27864583333333331</v>
+        <v>0.27577319587628868</v>
       </c>
       <c r="AM9" s="4">
         <f t="shared" si="4"/>
@@ -1766,11 +1772,11 @@
       </c>
       <c r="AK10" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL10" s="7">
         <f t="shared" si="3"/>
-        <v>0.72395833333333337</v>
+        <v>0.71649484536082486</v>
       </c>
       <c r="AM10" s="4">
         <f t="shared" si="4"/>
@@ -1885,11 +1891,11 @@
       </c>
       <c r="AK11" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL11" s="7">
         <f t="shared" si="3"/>
-        <v>0.48437499999999994</v>
+        <v>0.47938144329896903</v>
       </c>
       <c r="AM11" s="4">
         <f t="shared" si="4"/>
@@ -1960,13 +1966,15 @@
       <c r="Q12" s="1">
         <v>0.2</v>
       </c>
-      <c r="R12" s="1"/>
+      <c r="R12" s="1">
+        <v>0.4</v>
+      </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1">
         <f t="shared" si="0"/>
-        <v>6.7</v>
+        <v>7.1000000000000005</v>
       </c>
       <c r="W12" s="1">
         <v>0</v>
@@ -1985,22 +1993,24 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
+      <c r="AH12" s="1">
+        <v>0.1</v>
+      </c>
       <c r="AI12" s="1">
         <f t="shared" si="9"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="AJ12" s="1">
         <f t="shared" si="1"/>
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
       <c r="AK12" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL12" s="7">
         <f t="shared" si="3"/>
-        <v>0.35937500000000006</v>
+        <v>0.3814432989690722</v>
       </c>
       <c r="AM12" s="4">
         <f t="shared" si="4"/>
@@ -2117,11 +2127,11 @@
       </c>
       <c r="AK13" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL13" s="7">
         <f t="shared" si="3"/>
-        <v>0.34374999999999989</v>
+        <v>0.34020618556701021</v>
       </c>
       <c r="AM13" s="4">
         <f t="shared" si="4"/>
@@ -2248,11 +2258,11 @@
       </c>
       <c r="AK14" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL14" s="7">
         <f t="shared" si="3"/>
-        <v>0.61458333333333326</v>
+        <v>0.60824742268041232</v>
       </c>
       <c r="AM14" s="4">
         <f t="shared" si="4"/>
@@ -2264,28 +2274,30 @@
       <c r="AO14" s="1">
         <v>1</v>
       </c>
-      <c r="AP14" s="1"/>
+      <c r="AP14" s="1">
+        <v>1</v>
+      </c>
       <c r="AQ14" s="1">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AR14" s="1">
         <v>3</v>
       </c>
       <c r="AS14" s="4">
         <f t="shared" si="6"/>
-        <v>66.666666666666657</v>
+        <v>100</v>
       </c>
       <c r="AT14" s="4">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AU14" s="4">
         <v>0</v>
       </c>
       <c r="AV14" s="4">
         <f t="shared" si="8"/>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="AW14" s="5"/>
     </row>
@@ -2331,13 +2343,15 @@
       <c r="Q15" s="1">
         <v>0.6</v>
       </c>
-      <c r="R15" s="1"/>
+      <c r="R15" s="1">
+        <v>0.9</v>
+      </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1">
         <f t="shared" si="0"/>
-        <v>6.75</v>
+        <v>7.65</v>
       </c>
       <c r="W15" s="1">
         <v>0</v>
@@ -2361,15 +2375,15 @@
       </c>
       <c r="AJ15" s="1">
         <f t="shared" si="1"/>
-        <v>6.85</v>
+        <v>7.75</v>
       </c>
       <c r="AK15" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL15" s="7">
         <f t="shared" si="3"/>
-        <v>0.35677083333333331</v>
+        <v>0.39948453608247425</v>
       </c>
       <c r="AM15" s="4">
         <f t="shared" si="4"/>
@@ -2450,13 +2464,15 @@
       <c r="Q16" s="1">
         <v>0.7</v>
       </c>
-      <c r="R16" s="1"/>
+      <c r="R16" s="1">
+        <v>1.3</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1">
         <f t="shared" si="0"/>
-        <v>10.3</v>
+        <v>11.600000000000001</v>
       </c>
       <c r="W16" s="1">
         <v>0</v>
@@ -2480,19 +2496,19 @@
       </c>
       <c r="AJ16" s="1">
         <f t="shared" si="1"/>
-        <v>10.4</v>
+        <v>11.700000000000001</v>
       </c>
       <c r="AK16" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL16" s="7">
         <f t="shared" si="3"/>
-        <v>0.54166666666666674</v>
+        <v>0.60309278350515472</v>
       </c>
       <c r="AM16" s="4">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AN16" s="1">
         <v>0.5</v>
@@ -2521,7 +2537,7 @@
       </c>
       <c r="AV16" s="4">
         <f t="shared" si="8"/>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
       <c r="AW16" s="5"/>
     </row>
@@ -2603,11 +2619,11 @@
       </c>
       <c r="AK17" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL17" s="7">
         <f t="shared" si="3"/>
-        <v>0.47656250000000006</v>
+        <v>0.47164948453608252</v>
       </c>
       <c r="AM17" s="4">
         <f t="shared" si="4"/>
@@ -2708,11 +2724,11 @@
       </c>
       <c r="AK18" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL18" s="7">
         <f t="shared" si="3"/>
-        <v>0.26302083333333331</v>
+        <v>0.26030927835051548</v>
       </c>
       <c r="AM18" s="4">
         <f t="shared" si="4"/>
@@ -2787,15 +2803,17 @@
         <v>0.25</v>
       </c>
       <c r="Q19" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="R19" s="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0.8</v>
+      </c>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1">
         <f t="shared" si="0"/>
-        <v>7.7499999999999991</v>
+        <v>8.6499999999999986</v>
       </c>
       <c r="W19" s="1">
         <v>0.1</v>
@@ -2825,15 +2843,15 @@
       </c>
       <c r="AJ19" s="1">
         <f t="shared" si="1"/>
-        <v>8.35</v>
+        <v>9.2499999999999982</v>
       </c>
       <c r="AK19" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL19" s="7">
         <f t="shared" si="3"/>
-        <v>0.43489583333333331</v>
+        <v>0.47680412371134012</v>
       </c>
       <c r="AM19" s="4">
         <f t="shared" si="4"/>
@@ -2919,7 +2937,9 @@
       </c>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
+      <c r="U20" s="1">
+        <v>0.5</v>
+      </c>
       <c r="V20" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2953,22 +2973,24 @@
         <v>0.1</v>
       </c>
       <c r="AG20" s="1"/>
-      <c r="AH20" s="1"/>
+      <c r="AH20" s="1">
+        <v>0.2</v>
+      </c>
       <c r="AI20" s="1">
         <f t="shared" si="9"/>
-        <v>0.89999999999999991</v>
+        <v>1.0999999999999999</v>
       </c>
       <c r="AJ20" s="1">
         <f t="shared" si="1"/>
-        <v>17.899999999999999</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="AK20" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL20" s="7">
         <f t="shared" si="3"/>
-        <v>0.93229166666666663</v>
+        <v>0.93298969072164961</v>
       </c>
       <c r="AM20" s="4">
         <f t="shared" si="4"/>
@@ -3075,11 +3097,11 @@
       </c>
       <c r="AK21" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL21" s="7">
         <f t="shared" si="3"/>
-        <v>0.21354166666666666</v>
+        <v>0.21134020618556701</v>
       </c>
       <c r="AM21" s="4">
         <f t="shared" si="4"/>
@@ -3192,11 +3214,11 @@
       </c>
       <c r="AK22" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL22" s="7">
         <f t="shared" si="3"/>
-        <v>0.48437500000000006</v>
+        <v>0.47938144329896915</v>
       </c>
       <c r="AM22" s="4">
         <f t="shared" si="4"/>
@@ -3293,11 +3315,11 @@
       </c>
       <c r="AK23" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL23" s="7">
         <f t="shared" si="3"/>
-        <v>0.234375</v>
+        <v>0.23195876288659795</v>
       </c>
       <c r="AM23" s="4">
         <f t="shared" si="4"/>
@@ -3374,13 +3396,15 @@
       <c r="Q24" s="1">
         <v>1</v>
       </c>
-      <c r="R24" s="1"/>
+      <c r="R24" s="1">
+        <v>1.5</v>
+      </c>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1">
         <f t="shared" si="0"/>
-        <v>13.35</v>
+        <v>14.85</v>
       </c>
       <c r="W24" s="1">
         <v>0</v>
@@ -3407,26 +3431,28 @@
       <c r="AG24" s="1">
         <v>0.1</v>
       </c>
-      <c r="AH24" s="1"/>
+      <c r="AH24" s="1">
+        <v>0.1</v>
+      </c>
       <c r="AI24" s="1">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="AJ24" s="1">
         <f t="shared" si="1"/>
-        <v>13.95</v>
+        <v>15.549999999999999</v>
       </c>
       <c r="AK24" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL24" s="7">
         <f t="shared" si="3"/>
-        <v>0.7265625</v>
+        <v>0.80154639175257736</v>
       </c>
       <c r="AM24" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN24" s="1">
         <v>1</v>
@@ -3455,7 +3481,7 @@
       </c>
       <c r="AV24" s="4">
         <f t="shared" si="8"/>
-        <v>2.6666666666666665</v>
+        <v>3</v>
       </c>
       <c r="AW24" s="5"/>
     </row>
@@ -3521,11 +3547,11 @@
       </c>
       <c r="AK25" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL25" s="7">
         <f t="shared" si="3"/>
-        <v>0.2734375</v>
+        <v>0.27061855670103097</v>
       </c>
       <c r="AM25" s="4">
         <f t="shared" si="4"/>
@@ -3636,11 +3662,11 @@
       </c>
       <c r="AK26" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL26" s="7">
         <f t="shared" si="3"/>
-        <v>0.66666666666666674</v>
+        <v>0.65979381443298979</v>
       </c>
       <c r="AM26" s="4">
         <f t="shared" si="4"/>
@@ -3762,22 +3788,24 @@
       <c r="AG27" s="1">
         <v>0.2</v>
       </c>
-      <c r="AH27" s="1"/>
+      <c r="AH27" s="1">
+        <v>0.2</v>
+      </c>
       <c r="AI27" s="1">
         <f t="shared" si="9"/>
-        <v>1.6999999999999997</v>
+        <v>1.8999999999999997</v>
       </c>
       <c r="AJ27" s="1">
         <f t="shared" si="1"/>
-        <v>18.7</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="AK27" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL27" s="7">
         <f t="shared" si="3"/>
-        <v>0.97395833333333337</v>
+        <v>0.97422680412371132</v>
       </c>
       <c r="AM27" s="4">
         <f t="shared" si="4"/>
@@ -3883,22 +3911,24 @@
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
+      <c r="AH28" s="1">
+        <v>0.1</v>
+      </c>
       <c r="AI28" s="1">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="AJ28" s="1">
         <f t="shared" si="1"/>
-        <v>6.5499999999999989</v>
+        <v>6.6499999999999995</v>
       </c>
       <c r="AK28" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL28" s="7">
         <f t="shared" si="3"/>
-        <v>0.34114583333333331</v>
+        <v>0.34278350515463918</v>
       </c>
       <c r="AM28" s="4">
         <f t="shared" si="4"/>
@@ -4007,11 +4037,11 @@
       </c>
       <c r="AK29" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL29" s="7">
         <f t="shared" si="3"/>
-        <v>0.36718749999999994</v>
+        <v>0.36340206185567009</v>
       </c>
       <c r="AM29" s="4">
         <f t="shared" si="4"/>
@@ -4104,11 +4134,11 @@
       </c>
       <c r="AK30" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL30" s="7">
         <f t="shared" si="3"/>
-        <v>0.26041666666666669</v>
+        <v>0.25773195876288663</v>
       </c>
       <c r="AM30" s="4">
         <f t="shared" si="4"/>
@@ -4207,11 +4237,11 @@
       </c>
       <c r="AK31" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL31" s="7">
         <f t="shared" si="3"/>
-        <v>0.27083333333333337</v>
+        <v>0.26804123711340211</v>
       </c>
       <c r="AM31" s="4">
         <f t="shared" si="4"/>
@@ -4288,13 +4318,15 @@
       <c r="Q32" s="1">
         <v>1</v>
       </c>
-      <c r="R32" s="1"/>
+      <c r="R32" s="1">
+        <v>1</v>
+      </c>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1">
         <f t="shared" si="0"/>
-        <v>11.899999999999999</v>
+        <v>12.899999999999999</v>
       </c>
       <c r="W32" s="1">
         <v>0.2</v>
@@ -4324,15 +4356,15 @@
       </c>
       <c r="AJ32" s="1">
         <f t="shared" si="1"/>
-        <v>12.7</v>
+        <v>13.7</v>
       </c>
       <c r="AK32" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL32" s="7">
         <f t="shared" si="3"/>
-        <v>0.66145833333333337</v>
+        <v>0.70618556701030932</v>
       </c>
       <c r="AM32" s="4">
         <f t="shared" si="4"/>
@@ -4443,11 +4475,11 @@
       </c>
       <c r="AK33" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL33" s="7">
         <f t="shared" si="3"/>
-        <v>0.44531249999999994</v>
+        <v>0.44072164948453607</v>
       </c>
       <c r="AM33" s="4">
         <f t="shared" si="4"/>
@@ -4526,13 +4558,15 @@
       <c r="Q34" s="1">
         <v>1.25</v>
       </c>
-      <c r="R34" s="1"/>
+      <c r="R34" s="1">
+        <v>1.5</v>
+      </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1">
         <f t="shared" si="0"/>
-        <v>13.45</v>
+        <v>14.95</v>
       </c>
       <c r="W34" s="1">
         <v>0</v>
@@ -4555,22 +4589,24 @@
       <c r="AG34" s="1">
         <v>0.1</v>
       </c>
-      <c r="AH34" s="1"/>
+      <c r="AH34" s="1">
+        <v>0.1</v>
+      </c>
       <c r="AI34" s="1">
         <f t="shared" si="9"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AJ34" s="1">
         <f t="shared" si="1"/>
-        <v>13.85</v>
+        <v>15.45</v>
       </c>
       <c r="AK34" s="1">
         <f t="shared" si="2"/>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL34" s="7">
         <f t="shared" si="3"/>
-        <v>0.72135416666666663</v>
+        <v>0.79639175257731964</v>
       </c>
       <c r="AM34" s="4">
         <f t="shared" si="4"/>
@@ -4694,18 +4730,20 @@
       <c r="AG35" s="1">
         <v>0.2</v>
       </c>
-      <c r="AH35" s="1"/>
+      <c r="AH35" s="1">
+        <v>0.2</v>
+      </c>
       <c r="AI35" s="1">
         <f t="shared" si="9"/>
-        <v>2.1999999999999997</v>
+        <v>2.4</v>
       </c>
       <c r="AJ35" s="1">
         <f t="shared" ref="AJ35" si="10">V35+AI35</f>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AK35" s="4">
         <f>AJ35</f>
-        <v>19.2</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AL35" s="7">
         <f t="shared" ref="AL35" si="11">(AJ35/AK35)</f>

</xml_diff>